<commit_message>
Integrate Creation Club armors
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\Spreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C5F8BE-DFAC-4888-B78B-14C28AB0E95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F8B91F-12D2-4E98-B735-183775F7A33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
   <sheets>
     <sheet name="Armors" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="202">
   <si>
     <t>Amber</t>
   </si>
@@ -576,13 +576,82 @@
   </si>
   <si>
     <t>Light_ThievesGuildKarliah</t>
+  </si>
+  <si>
+    <t>Heavy_AncientDragonplate</t>
+  </si>
+  <si>
+    <t>Light_NetchLeather</t>
+  </si>
+  <si>
+    <t>Heavy_VvardenfellEbony</t>
+  </si>
+  <si>
+    <t>Light_AncientDragonscale</t>
+  </si>
+  <si>
+    <t>Heavy_DremoraPirate</t>
+  </si>
+  <si>
+    <t>Heavy_SilverHand</t>
+  </si>
+  <si>
+    <t>Heavy_TheSkinner</t>
+  </si>
+  <si>
+    <t>Light_EliteAlikr</t>
+  </si>
+  <si>
+    <t>Heavy_Tyranus</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Heavy_Chief</t>
+  </si>
+  <si>
+    <t>Heavy_Halvar</t>
+  </si>
+  <si>
+    <t>Light_Orcish</t>
+  </si>
+  <si>
+    <t>Heavy_SilverHandVeteran</t>
+  </si>
+  <si>
+    <t>Light_AlainElven</t>
+  </si>
+  <si>
+    <t>Light_ShadowedNetchLeather</t>
+  </si>
+  <si>
+    <t>Heavy_EbonySpellKnight</t>
+  </si>
+  <si>
+    <t>Heavy_SteelSpellKnight</t>
+  </si>
+  <si>
+    <t>Heavy_IronSpellKnight</t>
+  </si>
+  <si>
+    <t>Light_PaintedNetchLeather</t>
+  </si>
+  <si>
+    <t>AncientHelmetOfTheUnburned</t>
+  </si>
+  <si>
+    <t>Heavy_Stalhrim_Head</t>
+  </si>
+  <si>
+    <t>Heavy_AicantarDwarven</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -597,8 +666,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -641,6 +717,17 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -651,7 +738,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -659,8 +746,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
@@ -668,14 +758,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="9"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="10">
     <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
     <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
     <cellStyle name="60% - Accent3" xfId="3" builtinId="40"/>
     <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
     <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
     <cellStyle name="60% - Accent6" xfId="6" builtinId="52"/>
+    <cellStyle name="60% - AccentRed" xfId="8" xr:uid="{2BFDBC86-946D-4F9C-9D98-E6A31F9B39D6}"/>
+    <cellStyle name="Accent1" xfId="7" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="9" builtinId="41"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -988,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,58 +1150,51 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="3">
-        <v>600</v>
-      </c>
-      <c r="C3" s="3">
-        <v>50</v>
-      </c>
-      <c r="D3" s="3">
-        <v>300</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="A3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>250</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="s">
-        <v>162</v>
+      <c r="I3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="3">
-        <v>600</v>
-      </c>
-      <c r="C4" s="3">
-        <v>50</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4">
         <v>500</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>250</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3">
         <v>600</v>
@@ -1115,7 +1203,7 @@
         <v>50</v>
       </c>
       <c r="D5" s="3">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>11</v>
@@ -1128,12 +1216,12 @@
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B6" s="3">
         <v>600</v>
@@ -1144,23 +1232,19 @@
       <c r="D6" s="3">
         <v>500</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="I6" s="3" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>68</v>
+        <v>190</v>
       </c>
       <c r="B7" s="3">
         <v>600</v>
@@ -1182,190 +1266,199 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="3">
+        <v>600</v>
+      </c>
+      <c r="C8" s="3">
+        <v>50</v>
+      </c>
+      <c r="D8" s="3">
+        <v>500</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" s="3">
+        <v>600</v>
+      </c>
+      <c r="C9" s="3">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3">
+        <v>500</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10" s="3">
+        <v>600</v>
+      </c>
+      <c r="C10" s="3">
+        <v>50</v>
+      </c>
+      <c r="D10" s="3">
+        <v>500</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="3">
+        <v>600</v>
+      </c>
+      <c r="C11" s="3">
+        <v>50</v>
+      </c>
+      <c r="D11" s="3">
+        <v>500</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B12" s="3">
+        <v>600</v>
+      </c>
+      <c r="C12" s="3">
+        <v>50</v>
+      </c>
+      <c r="D12" s="3">
+        <v>500</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="3">
+        <v>600</v>
+      </c>
+      <c r="C13" s="3">
+        <v>50</v>
+      </c>
+      <c r="D13" s="3">
+        <v>500</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>51</v>
       </c>
-      <c r="B8">
+      <c r="B14">
         <v>600</v>
       </c>
-      <c r="C8">
+      <c r="C14">
         <v>40</v>
       </c>
-      <c r="D8">
+      <c r="D14">
         <v>1000</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E14" t="s">
         <v>72</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F14" t="s">
         <v>9</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G14" t="s">
         <v>10</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I14" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="4">
-        <v>700</v>
-      </c>
-      <c r="C9" s="4">
-        <v>50</v>
-      </c>
-      <c r="D9" s="4">
-        <v>5000</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="4">
-        <v>700</v>
-      </c>
-      <c r="C10" s="4">
-        <v>50</v>
-      </c>
-      <c r="D10" s="4">
-        <v>2500</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="4">
-        <v>700</v>
-      </c>
-      <c r="C11" s="4">
-        <v>50</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1000</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="4">
-        <v>700</v>
-      </c>
-      <c r="C12" s="4">
-        <v>50</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1000</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13">
-        <v>700</v>
-      </c>
-      <c r="C13">
-        <v>50</v>
-      </c>
-      <c r="D13">
-        <v>1500</v>
-      </c>
-      <c r="E13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="2">
-        <v>800</v>
-      </c>
-      <c r="C14" s="2">
-        <v>60</v>
-      </c>
-      <c r="D14" s="2">
-        <v>400</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="C15" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D15" s="2">
-        <v>400</v>
+        <v>5000</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>144</v>
@@ -1373,98 +1466,82 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B16" s="2">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="C16" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D16" s="2">
-        <v>1000</v>
-      </c>
-      <c r="E16" s="2" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="I16" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B17" s="2">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="C17" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D17" s="2">
-        <v>1500</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" s="2"/>
+        <v>1000</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="I17" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B18" s="2">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="C18" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D18" s="2">
         <v>1000</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="I18" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>69</v>
+        <v>185</v>
       </c>
       <c r="B19" s="2">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="C19" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D19" s="2">
         <v>1000</v>
@@ -1473,1041 +1550,1533 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20">
-        <v>800</v>
-      </c>
-      <c r="C20">
+      <c r="A20" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" s="2">
+        <v>700</v>
+      </c>
+      <c r="C20" s="2">
         <v>50</v>
       </c>
-      <c r="D20">
-        <v>5000</v>
-      </c>
-      <c r="H20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="D20" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>142</v>
       </c>
       <c r="B21">
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="C21">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="D21">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F21" t="s">
         <v>9</v>
       </c>
       <c r="G21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="5">
+        <v>800</v>
+      </c>
+      <c r="C22" s="5">
+        <v>60</v>
+      </c>
+      <c r="D22" s="5">
+        <v>400</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="5">
+        <v>800</v>
+      </c>
+      <c r="C23" s="5">
+        <v>60</v>
+      </c>
+      <c r="D23" s="5">
+        <v>400</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="5">
+        <v>800</v>
+      </c>
+      <c r="C24" s="5">
+        <v>60</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1000</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I21" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="1">
+      <c r="H24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="5">
+        <v>800</v>
+      </c>
+      <c r="C25" s="5">
+        <v>60</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1500</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="5">
+        <v>800</v>
+      </c>
+      <c r="C26" s="5">
+        <v>60</v>
+      </c>
+      <c r="D26" s="5">
         <v>1000</v>
       </c>
-      <c r="C22" s="1">
-        <v>80</v>
-      </c>
-      <c r="D22" s="1">
-        <v>20000</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C23" s="1">
-        <v>80</v>
-      </c>
-      <c r="D23" s="1">
-        <v>10000</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1" t="s">
+      <c r="E26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C24" s="1">
-        <v>80</v>
-      </c>
-      <c r="D24" s="1">
-        <v>10000</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C25" s="1">
-        <v>80</v>
-      </c>
-      <c r="D25" s="1">
-        <v>10000</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26">
-        <v>1000</v>
-      </c>
-      <c r="C26">
-        <v>70</v>
-      </c>
-      <c r="D26">
-        <v>20000</v>
-      </c>
-      <c r="E26" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26" t="s">
-        <v>5</v>
-      </c>
-      <c r="I26" t="s">
-        <v>160</v>
+      <c r="H26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B27">
-        <v>1200</v>
+        <v>800</v>
       </c>
       <c r="C27">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D27">
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="H27" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="I27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="B28">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="C28">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D28">
-        <v>50000</v>
+        <v>2000</v>
+      </c>
+      <c r="H28" t="s">
+        <v>76</v>
+      </c>
+      <c r="I28" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>201</v>
       </c>
       <c r="B29">
-        <v>250</v>
+        <v>900</v>
       </c>
       <c r="C29">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="D29">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="H29" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="I29" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="B30">
-        <v>250</v>
+        <v>900</v>
       </c>
       <c r="C30">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="D30">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="E30" t="s">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="F30" t="s">
+        <v>9</v>
       </c>
       <c r="G30" t="s">
         <v>5</v>
       </c>
       <c r="I30" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B31" s="8">
+        <v>900</v>
+      </c>
+      <c r="C31" s="8">
+        <v>70</v>
+      </c>
+      <c r="D31" s="8">
+        <v>20000</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C32" s="1">
+        <v>80</v>
+      </c>
+      <c r="D32" s="1">
+        <v>20000</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C33" s="1">
+        <v>80</v>
+      </c>
+      <c r="D33" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C34" s="1">
+        <v>80</v>
+      </c>
+      <c r="D34" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C35" s="1">
+        <v>80</v>
+      </c>
+      <c r="D35" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C36" s="1">
+        <v>80</v>
+      </c>
+      <c r="D36" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C37" s="1">
+        <v>80</v>
+      </c>
+      <c r="D37" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C38" s="8">
+        <v>70</v>
+      </c>
+      <c r="D38" s="8">
+        <v>20000</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="7">
+        <v>1200</v>
+      </c>
+      <c r="C39" s="7">
+        <v>100</v>
+      </c>
+      <c r="D39" s="7">
+        <v>50000</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="7">
+        <v>1200</v>
+      </c>
+      <c r="C40" s="7">
+        <v>100</v>
+      </c>
+      <c r="D40" s="7">
+        <v>50000</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B41" s="7">
+        <v>1200</v>
+      </c>
+      <c r="C41" s="7">
+        <v>100</v>
+      </c>
+      <c r="D41" s="7">
+        <v>50000</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42">
+        <v>250</v>
+      </c>
+      <c r="C42">
+        <v>8</v>
+      </c>
+      <c r="D42">
+        <v>100</v>
+      </c>
+      <c r="H42" t="s">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43">
+        <v>250</v>
+      </c>
+      <c r="C43">
+        <v>8</v>
+      </c>
+      <c r="D43">
+        <v>100</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1</v>
+      </c>
+      <c r="G43" t="s">
+        <v>5</v>
+      </c>
+      <c r="I43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B44" s="4">
         <v>300</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C44" s="4">
         <v>10</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D44" s="4">
         <v>300</v>
       </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5" t="s">
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I31" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="I44" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B45" s="4">
         <v>300</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C45" s="4">
         <v>10</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D45" s="4">
         <v>200</v>
       </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5" t="s">
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I32" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="I45" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B46" s="4">
         <v>300</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C46" s="4">
         <v>10</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D46" s="4">
         <v>200</v>
       </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5" t="s">
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I33" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="I46" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B47" s="4">
         <v>300</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C47" s="4">
         <v>10</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D47" s="4">
         <v>200</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E47" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F47" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G47" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="H47" s="4"/>
+      <c r="I47" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B48" s="4">
         <v>300</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C48" s="4">
         <v>10</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D48" s="4">
         <v>200</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E48" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F48" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G48" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="H48" s="4"/>
+      <c r="I48" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B49" s="4">
         <v>300</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C49" s="4">
         <v>10</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D49" s="4">
         <v>200</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E49" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F49" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="G49" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="H49" s="4"/>
+      <c r="I49" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B50" s="4">
         <v>300</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C50" s="4">
         <v>10</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D50" s="4">
         <v>200</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5" t="s">
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I37" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="I50" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B51" s="4">
+        <v>300</v>
+      </c>
+      <c r="C51" s="4">
+        <v>10</v>
+      </c>
+      <c r="D51" s="4">
+        <v>400</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B52" s="4">
+        <v>300</v>
+      </c>
+      <c r="C52" s="4">
+        <v>10</v>
+      </c>
+      <c r="D52" s="4">
+        <v>400</v>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B53" s="4">
+        <v>300</v>
+      </c>
+      <c r="C53" s="4">
+        <v>10</v>
+      </c>
+      <c r="D53" s="4">
+        <v>400</v>
+      </c>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B54" s="4">
         <v>300</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C54" s="4">
         <v>10</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D54" s="4">
         <v>200</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5" t="s">
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I38" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="I54" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B55" s="4">
         <v>300</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C55" s="4">
         <v>10</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D55" s="4">
         <v>400</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5" t="s">
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I39" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="I55" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B56" s="4">
         <v>300</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C56" s="4">
         <v>10</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D56" s="4">
         <v>200</v>
       </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5" t="s">
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I40" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="I56" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B57" s="4">
         <v>300</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C57" s="4">
         <v>10</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D57" s="4">
         <v>200</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5" t="s">
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="I57" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B58" s="4">
         <v>300</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C58" s="4">
         <v>10</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D58" s="4">
         <v>200</v>
       </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B59" s="4">
         <v>300</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C59" s="4">
         <v>10</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D59" s="4">
         <v>200</v>
       </c>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5" t="s">
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I43" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="I59" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B60" s="4">
         <v>300</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C60" s="4">
         <v>10</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D60" s="4">
         <v>200</v>
       </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5" t="s">
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I44" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="I60" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>29</v>
       </c>
-      <c r="B45">
+      <c r="B61">
         <v>300</v>
       </c>
-      <c r="C45">
+      <c r="C61">
         <v>15</v>
       </c>
-      <c r="D45">
+      <c r="D61">
         <v>400</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H61" t="s">
         <v>1</v>
       </c>
-      <c r="I45" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="I61" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>83</v>
       </c>
-      <c r="B46">
+      <c r="B62">
         <v>300</v>
       </c>
-      <c r="C46">
+      <c r="C62">
         <v>15</v>
       </c>
-      <c r="D46">
+      <c r="D62">
         <v>400</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H62" t="s">
         <v>1</v>
       </c>
-      <c r="I46" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+      <c r="I62" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B63" s="6">
         <v>350</v>
       </c>
-      <c r="C47" s="6">
+      <c r="C63" s="6">
         <v>12</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D63" s="6">
         <v>400</v>
       </c>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6" t="s">
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I47" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+      <c r="I63" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B64" s="6">
+        <v>350</v>
+      </c>
+      <c r="C64" s="6">
+        <v>12</v>
+      </c>
+      <c r="D64" s="6">
+        <v>400</v>
+      </c>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B65" s="6">
         <v>350</v>
       </c>
-      <c r="C48" s="6">
+      <c r="C65" s="6">
         <v>12</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D65" s="6">
         <v>10000</v>
       </c>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6" t="s">
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I48" s="6" t="s">
+      <c r="I65" s="6" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B66" s="6">
         <v>350</v>
       </c>
-      <c r="C49" s="6">
+      <c r="C66" s="6">
         <v>12</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D66" s="6">
         <v>1000</v>
       </c>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6" t="s">
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I49" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+      <c r="I66" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67">
+        <v>400</v>
+      </c>
+      <c r="C67">
+        <v>20</v>
+      </c>
+      <c r="D67">
+        <v>800</v>
+      </c>
+      <c r="E67" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67" t="s">
+        <v>10</v>
+      </c>
+      <c r="I67" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B68" s="5">
+        <v>400</v>
+      </c>
+      <c r="C68" s="5">
+        <v>15</v>
+      </c>
+      <c r="D68" s="5">
+        <v>800</v>
+      </c>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" s="5">
+        <v>400</v>
+      </c>
+      <c r="C69" s="5">
+        <v>15</v>
+      </c>
+      <c r="D69" s="5">
+        <v>800</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>25</v>
+      </c>
+      <c r="B70">
+        <v>400</v>
+      </c>
+      <c r="C70">
+        <v>20</v>
+      </c>
+      <c r="D70">
+        <v>100</v>
+      </c>
+      <c r="H70" t="s">
+        <v>14</v>
+      </c>
+      <c r="I70" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>37</v>
+      </c>
+      <c r="B71">
+        <v>450</v>
+      </c>
+      <c r="C71">
+        <v>35</v>
+      </c>
+      <c r="D71">
+        <v>1000</v>
+      </c>
+      <c r="E71" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G71" t="s">
+        <v>10</v>
+      </c>
+      <c r="I71" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>21</v>
+      </c>
+      <c r="B72">
+        <v>500</v>
+      </c>
+      <c r="C72">
+        <v>30</v>
+      </c>
+      <c r="D72">
+        <v>600</v>
+      </c>
+      <c r="H72" t="s">
+        <v>11</v>
+      </c>
+      <c r="I72" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73">
+        <v>500</v>
+      </c>
+      <c r="C73">
+        <v>30</v>
+      </c>
+      <c r="D73">
+        <v>5000</v>
+      </c>
+      <c r="H73" t="s">
+        <v>8</v>
+      </c>
+      <c r="I73" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>191</v>
+      </c>
+      <c r="B74">
+        <v>500</v>
+      </c>
+      <c r="C74">
+        <v>30</v>
+      </c>
+      <c r="D74">
+        <v>1000</v>
+      </c>
+      <c r="E74" t="s">
+        <v>76</v>
+      </c>
+      <c r="F74" t="s">
+        <v>9</v>
+      </c>
+      <c r="G74" t="s">
+        <v>5</v>
+      </c>
+      <c r="I74" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>36</v>
+      </c>
+      <c r="B75">
+        <v>500</v>
+      </c>
+      <c r="C75">
+        <v>15</v>
+      </c>
+      <c r="D75">
+        <v>600</v>
+      </c>
+      <c r="H75" t="s">
+        <v>1</v>
+      </c>
+      <c r="I75" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>38</v>
+      </c>
+      <c r="B76">
+        <v>500</v>
+      </c>
+      <c r="C76">
+        <v>20</v>
+      </c>
+      <c r="D76">
+        <v>400</v>
+      </c>
+      <c r="E76" t="s">
+        <v>11</v>
+      </c>
+      <c r="F76" t="s">
+        <v>16</v>
+      </c>
+      <c r="G76" t="s">
+        <v>5</v>
+      </c>
+      <c r="I76" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>41</v>
+      </c>
+      <c r="B77">
+        <v>500</v>
+      </c>
+      <c r="C77">
+        <v>15</v>
+      </c>
+      <c r="D77">
+        <v>8000</v>
+      </c>
+      <c r="H77" t="s">
+        <v>7</v>
+      </c>
+      <c r="I77" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B78" s="8">
+        <v>500</v>
+      </c>
+      <c r="C78" s="8">
+        <v>30</v>
+      </c>
+      <c r="D78" s="8">
+        <v>16000</v>
+      </c>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I78" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79" s="1">
+        <v>550</v>
+      </c>
+      <c r="C79" s="1">
+        <v>25</v>
+      </c>
+      <c r="D79" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B80" s="1">
+        <v>550</v>
+      </c>
+      <c r="C80" s="1">
+        <v>25</v>
+      </c>
+      <c r="D80" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B81" s="1">
+        <v>550</v>
+      </c>
+      <c r="C81" s="1">
+        <v>25</v>
+      </c>
+      <c r="D81" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="6">
-        <v>350</v>
-      </c>
-      <c r="C50" s="6">
+      <c r="B82" s="1">
+        <v>550</v>
+      </c>
+      <c r="C82" s="1">
+        <v>25</v>
+      </c>
+      <c r="D82" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B83" s="8">
+        <v>600</v>
+      </c>
+      <c r="C83" s="8">
+        <v>30</v>
+      </c>
+      <c r="D83" s="8">
+        <v>16000</v>
+      </c>
+      <c r="E83" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D50" s="6">
-        <v>5000</v>
-      </c>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I50" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>20</v>
-      </c>
-      <c r="B51">
-        <v>400</v>
-      </c>
-      <c r="C51">
-        <v>20</v>
-      </c>
-      <c r="D51">
-        <v>800</v>
-      </c>
-      <c r="E51" t="s">
-        <v>8</v>
-      </c>
-      <c r="F51" t="s">
+      <c r="F83" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G51" t="s">
-        <v>10</v>
-      </c>
-      <c r="I51" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>23</v>
-      </c>
-      <c r="B52">
-        <v>400</v>
-      </c>
-      <c r="C52">
-        <v>15</v>
-      </c>
-      <c r="D52">
-        <v>800</v>
-      </c>
-      <c r="E52" t="s">
-        <v>7</v>
-      </c>
-      <c r="F52" t="s">
-        <v>13</v>
-      </c>
-      <c r="G52" t="s">
+      <c r="G83" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I52" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B53">
-        <v>400</v>
-      </c>
-      <c r="C53">
-        <v>20</v>
-      </c>
-      <c r="D53">
-        <v>100</v>
-      </c>
-      <c r="H53" t="s">
-        <v>14</v>
-      </c>
-      <c r="I53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>37</v>
-      </c>
-      <c r="B54">
-        <v>450</v>
-      </c>
-      <c r="C54">
-        <v>35</v>
-      </c>
-      <c r="D54">
-        <v>1000</v>
-      </c>
-      <c r="E54" t="s">
-        <v>8</v>
-      </c>
-      <c r="F54" t="s">
-        <v>9</v>
-      </c>
-      <c r="G54" t="s">
-        <v>10</v>
-      </c>
-      <c r="I54" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>21</v>
-      </c>
-      <c r="B55">
-        <v>500</v>
-      </c>
-      <c r="C55">
-        <v>30</v>
-      </c>
-      <c r="D55">
-        <v>600</v>
-      </c>
-      <c r="H55" t="s">
-        <v>11</v>
-      </c>
-      <c r="I55" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>34</v>
-      </c>
-      <c r="B56">
-        <v>500</v>
-      </c>
-      <c r="C56">
-        <v>30</v>
-      </c>
-      <c r="D56">
-        <v>5000</v>
-      </c>
-      <c r="H56" t="s">
-        <v>8</v>
-      </c>
-      <c r="I56" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>36</v>
-      </c>
-      <c r="B57">
-        <v>500</v>
-      </c>
-      <c r="C57">
-        <v>15</v>
-      </c>
-      <c r="D57">
-        <v>600</v>
-      </c>
-      <c r="H57" t="s">
-        <v>1</v>
-      </c>
-      <c r="I57" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>38</v>
-      </c>
-      <c r="B58">
-        <v>500</v>
-      </c>
-      <c r="C58">
-        <v>20</v>
-      </c>
-      <c r="D58">
-        <v>400</v>
-      </c>
-      <c r="E58" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" t="s">
-        <v>16</v>
-      </c>
-      <c r="G58" t="s">
-        <v>5</v>
-      </c>
-      <c r="I58" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>41</v>
-      </c>
-      <c r="B59">
-        <v>500</v>
-      </c>
-      <c r="C59">
-        <v>15</v>
-      </c>
-      <c r="D59">
-        <v>8000</v>
-      </c>
-      <c r="H59" t="s">
-        <v>7</v>
-      </c>
-      <c r="I59" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B60" s="1">
-        <v>550</v>
-      </c>
-      <c r="C60" s="1">
-        <v>25</v>
-      </c>
-      <c r="D60" s="1">
-        <v>6000</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B61" s="1">
-        <v>550</v>
-      </c>
-      <c r="C61" s="1">
-        <v>25</v>
-      </c>
-      <c r="D61" s="1">
-        <v>6000</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B62" s="1">
-        <v>550</v>
-      </c>
-      <c r="C62" s="1">
-        <v>25</v>
-      </c>
-      <c r="D62" s="1">
-        <v>6000</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>22</v>
-      </c>
-      <c r="B63">
-        <v>600</v>
-      </c>
-      <c r="C63">
-        <v>30</v>
-      </c>
-      <c r="D63">
-        <v>16000</v>
-      </c>
-      <c r="E63" t="s">
-        <v>12</v>
-      </c>
-      <c r="F63" t="s">
-        <v>9</v>
-      </c>
-      <c r="G63" t="s">
-        <v>5</v>
-      </c>
-      <c r="I63" t="s">
+      <c r="H83" s="8"/>
+      <c r="I83" s="8" t="s">
         <v>161</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A30:I63">
-    <sortCondition ref="B29:B63"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A43:I83">
+    <sortCondition ref="B42:B83"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2789,15 +3358,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B796E76-FF31-432C-A859-43C3EAF890A5}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="9.140625" customWidth="1"/>
   </cols>
@@ -2869,141 +3438,138 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>199</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E8">
-        <v>80000</v>
+        <v>5000</v>
       </c>
       <c r="F8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="B9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="E9">
+        <v>80000</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>105</v>
-      </c>
-      <c r="B21" t="s">
-        <v>130</v>
-      </c>
-      <c r="E21">
-        <v>80000</v>
-      </c>
-      <c r="F21" t="b">
-        <v>1</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="B22" t="s">
+        <v>130</v>
+      </c>
+      <c r="E22">
+        <v>80000</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>110</v>
-      </c>
-      <c r="B26" t="s">
-        <v>134</v>
-      </c>
-      <c r="C26">
-        <v>50</v>
-      </c>
-      <c r="E26">
-        <v>5000</v>
-      </c>
-      <c r="F26" t="b">
-        <v>0</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D27">
-        <v>-4</v>
+        <v>134</v>
+      </c>
+      <c r="C27">
+        <v>50</v>
       </c>
       <c r="E27">
         <v>5000</v>
@@ -3014,89 +3580,92 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="B28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28">
+        <v>-4</v>
+      </c>
+      <c r="E28">
+        <v>5000</v>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>120</v>
-      </c>
-      <c r="B36" t="s">
-        <v>136</v>
-      </c>
-      <c r="E36">
-        <v>80000</v>
-      </c>
-      <c r="F36" t="b">
-        <v>1</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="B37" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37">
+        <v>80000</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>122</v>
-      </c>
-      <c r="B38" t="s">
-        <v>137</v>
-      </c>
-      <c r="C38">
-        <v>25</v>
-      </c>
-      <c r="E38">
-        <v>5000</v>
-      </c>
-      <c r="F38" t="b">
-        <v>0</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B39" t="s">
-        <v>138</v>
+        <v>137</v>
+      </c>
+      <c r="C39">
+        <v>25</v>
       </c>
       <c r="E39">
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
@@ -3104,51 +3673,65 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="E40">
-        <v>80000</v>
+        <v>50000</v>
       </c>
       <c r="F40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>125</v>
+        <v>124</v>
+      </c>
+      <c r="B41" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41">
+        <v>50</v>
+      </c>
+      <c r="E41">
+        <v>80000</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>126</v>
-      </c>
-      <c r="B42" t="s">
-        <v>140</v>
-      </c>
-      <c r="E42">
-        <v>300</v>
-      </c>
-      <c r="F42" t="b">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" t="s">
+        <v>140</v>
+      </c>
+      <c r="E43">
+        <v>300</v>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>127</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>141</v>
       </c>
-      <c r="E43">
+      <c r="E44">
         <v>5000</v>
       </c>
-      <c r="F43" t="b">
+      <c r="F44" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Integrate Dwarven light armor
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6B89A2-16C1-46E7-98A0-8F56CA5BCA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC51DD9-4B26-48FE-99B7-785A1F8E95BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="203">
   <si>
     <t>Amber</t>
   </si>
@@ -645,6 +645,9 @@
   </si>
   <si>
     <t>Heavy_Chieftain</t>
+  </si>
+  <si>
+    <t>Light_Dwarven</t>
   </si>
 </sst>
 </file>
@@ -1083,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2741,73 +2744,79 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>25</v>
+        <v>202</v>
       </c>
       <c r="B70">
         <v>400</v>
       </c>
       <c r="C70">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D70">
-        <v>100</v>
-      </c>
-      <c r="H70" t="s">
-        <v>14</v>
+        <v>1000</v>
+      </c>
+      <c r="E70" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" t="s">
+        <v>1</v>
+      </c>
+      <c r="G70" t="s">
+        <v>5</v>
       </c>
       <c r="I70" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B71">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="C71">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D71">
-        <v>1000</v>
-      </c>
-      <c r="E71" t="s">
-        <v>8</v>
-      </c>
-      <c r="F71" t="s">
-        <v>9</v>
-      </c>
-      <c r="G71" t="s">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="H71" t="s">
+        <v>14</v>
       </c>
       <c r="I71" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B72">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="C72">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D72">
-        <v>600</v>
-      </c>
-      <c r="H72" t="s">
-        <v>11</v>
+        <v>1000</v>
+      </c>
+      <c r="E72" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72" t="s">
+        <v>10</v>
       </c>
       <c r="I72" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B73">
         <v>500</v>
@@ -2816,10 +2825,10 @@
         <v>30</v>
       </c>
       <c r="D73">
-        <v>5000</v>
+        <v>600</v>
       </c>
       <c r="H73" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I73" t="s">
         <v>144</v>
@@ -2827,7 +2836,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>190</v>
+        <v>34</v>
       </c>
       <c r="B74">
         <v>500</v>
@@ -2836,140 +2845,133 @@
         <v>30</v>
       </c>
       <c r="D74">
-        <v>1000</v>
-      </c>
-      <c r="E74" t="s">
-        <v>76</v>
-      </c>
-      <c r="F74" t="s">
-        <v>9</v>
-      </c>
-      <c r="G74" t="s">
-        <v>5</v>
+        <v>5000</v>
+      </c>
+      <c r="H74" t="s">
+        <v>8</v>
       </c>
       <c r="I74" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>36</v>
+        <v>190</v>
       </c>
       <c r="B75">
         <v>500</v>
       </c>
       <c r="C75">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D75">
-        <v>600</v>
-      </c>
-      <c r="H75" t="s">
-        <v>1</v>
+        <v>1000</v>
+      </c>
+      <c r="E75" t="s">
+        <v>76</v>
+      </c>
+      <c r="F75" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" t="s">
+        <v>5</v>
       </c>
       <c r="I75" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B76">
         <v>500</v>
       </c>
       <c r="C76">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D76">
-        <v>400</v>
-      </c>
-      <c r="E76" t="s">
-        <v>11</v>
-      </c>
-      <c r="F76" t="s">
-        <v>16</v>
-      </c>
-      <c r="G76" t="s">
-        <v>5</v>
+        <v>600</v>
+      </c>
+      <c r="H76" t="s">
+        <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B77">
         <v>500</v>
       </c>
       <c r="C77">
+        <v>20</v>
+      </c>
+      <c r="D77">
+        <v>400</v>
+      </c>
+      <c r="E77" t="s">
+        <v>11</v>
+      </c>
+      <c r="F77" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" t="s">
+        <v>5</v>
+      </c>
+      <c r="I77" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>41</v>
+      </c>
+      <c r="B78">
+        <v>500</v>
+      </c>
+      <c r="C78">
         <v>15</v>
       </c>
-      <c r="D77">
+      <c r="D78">
         <v>8000</v>
       </c>
-      <c r="H77" t="s">
+      <c r="H78" t="s">
         <v>7</v>
       </c>
-      <c r="I77" t="s">
+      <c r="I78" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B78" s="8">
+      <c r="B79" s="8">
         <v>500</v>
       </c>
-      <c r="C78" s="8">
+      <c r="C79" s="8">
         <v>30</v>
       </c>
-      <c r="D78" s="8">
+      <c r="D79" s="8">
         <v>16000</v>
       </c>
-      <c r="E78" s="8"/>
-      <c r="F78" s="8"/>
-      <c r="G78" s="8"/>
-      <c r="H78" s="8" t="s">
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I78" s="8" t="s">
+      <c r="I79" s="8" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B79" s="1">
-        <v>550</v>
-      </c>
-      <c r="C79" s="1">
-        <v>25</v>
-      </c>
-      <c r="D79" s="1">
-        <v>6000</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B80" s="1">
         <v>550</v>
@@ -2981,7 +2983,7 @@
         <v>6000</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>7</v>
@@ -2991,12 +2993,12 @@
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B81" s="1">
         <v>550</v>
@@ -3008,22 +3010,22 @@
         <v>6000</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B82" s="1">
         <v>550</v>
@@ -3034,46 +3036,73 @@
       <c r="D82" s="1">
         <v>6000</v>
       </c>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1" t="s">
+      <c r="E82" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F82" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H82" s="1"/>
       <c r="I82" s="1" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B83" s="1">
+        <v>550</v>
+      </c>
+      <c r="C83" s="1">
+        <v>25</v>
+      </c>
+      <c r="D83" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B83" s="8">
+      <c r="B84" s="8">
         <v>600</v>
       </c>
-      <c r="C83" s="8">
+      <c r="C84" s="8">
         <v>30</v>
       </c>
-      <c r="D83" s="8">
+      <c r="D84" s="8">
         <v>16000</v>
       </c>
-      <c r="E83" s="8" t="s">
+      <c r="E84" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F83" s="8" t="s">
+      <c r="F84" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G83" s="8" t="s">
+      <c r="G84" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H83" s="8"/>
-      <c r="I83" s="8" t="s">
+      <c r="H84" s="8"/>
+      <c r="I84" s="8" t="s">
         <v>161</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A43:I83">
-    <sortCondition ref="B42:B83"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A43:I84">
+    <sortCondition ref="B42:B84"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Orcish light armor requires pure orichalcum
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC51DD9-4B26-48FE-99B7-785A1F8E95BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A63B9EE-72D3-445E-A7DB-2008848A80A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2871,7 +2871,7 @@
         <v>76</v>
       </c>
       <c r="F75" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G75" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Set stats and recipes
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF969A7-8E73-44F0-B0A7-704925D134B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FA9EED-CA96-4AF4-A721-DAA5E8FBB21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="203">
   <si>
     <t>Amber</t>
   </si>
@@ -645,6 +645,9 @@
   </si>
   <si>
     <t>Light_Dwarven</t>
+  </si>
+  <si>
+    <t>Light_Chainmail</t>
   </si>
 </sst>
 </file>
@@ -1083,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="P64" sqref="P64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2715,7 +2718,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B69">
         <v>400</v>
@@ -2724,90 +2727,99 @@
         <v>30</v>
       </c>
       <c r="D69">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="E69" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="F69" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G69" t="s">
         <v>5</v>
       </c>
+      <c r="H69" t="s">
+        <v>16</v>
+      </c>
       <c r="I69" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>25</v>
+        <v>201</v>
       </c>
       <c r="B70">
         <v>400</v>
       </c>
       <c r="C70">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D70">
-        <v>100</v>
-      </c>
-      <c r="H70" t="s">
-        <v>14</v>
+        <v>1000</v>
+      </c>
+      <c r="E70" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" t="s">
+        <v>1</v>
+      </c>
+      <c r="G70" t="s">
+        <v>5</v>
       </c>
       <c r="I70" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B71">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="C71">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D71">
-        <v>1000</v>
-      </c>
-      <c r="E71" t="s">
-        <v>8</v>
-      </c>
-      <c r="F71" t="s">
-        <v>9</v>
-      </c>
-      <c r="G71" t="s">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="H71" t="s">
+        <v>14</v>
       </c>
       <c r="I71" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B72">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="C72">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D72">
-        <v>600</v>
-      </c>
-      <c r="H72" t="s">
-        <v>11</v>
+        <v>1000</v>
+      </c>
+      <c r="E72" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72" t="s">
+        <v>10</v>
       </c>
       <c r="I72" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B73">
         <v>500</v>
@@ -2816,10 +2828,10 @@
         <v>30</v>
       </c>
       <c r="D73">
-        <v>5000</v>
+        <v>600</v>
       </c>
       <c r="H73" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I73" t="s">
         <v>144</v>
@@ -2827,7 +2839,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>189</v>
+        <v>34</v>
       </c>
       <c r="B74">
         <v>500</v>
@@ -2836,140 +2848,133 @@
         <v>30</v>
       </c>
       <c r="D74">
-        <v>1000</v>
-      </c>
-      <c r="E74" t="s">
-        <v>76</v>
-      </c>
-      <c r="F74" t="s">
-        <v>1</v>
-      </c>
-      <c r="G74" t="s">
-        <v>5</v>
+        <v>5000</v>
+      </c>
+      <c r="H74" t="s">
+        <v>8</v>
       </c>
       <c r="I74" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>36</v>
+        <v>189</v>
       </c>
       <c r="B75">
         <v>500</v>
       </c>
       <c r="C75">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D75">
-        <v>600</v>
-      </c>
-      <c r="H75" t="s">
+        <v>1000</v>
+      </c>
+      <c r="E75" t="s">
+        <v>76</v>
+      </c>
+      <c r="F75" t="s">
         <v>1</v>
       </c>
+      <c r="G75" t="s">
+        <v>5</v>
+      </c>
       <c r="I75" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B76">
         <v>500</v>
       </c>
       <c r="C76">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D76">
-        <v>400</v>
-      </c>
-      <c r="E76" t="s">
-        <v>11</v>
-      </c>
-      <c r="F76" t="s">
-        <v>16</v>
-      </c>
-      <c r="G76" t="s">
-        <v>5</v>
+        <v>600</v>
+      </c>
+      <c r="H76" t="s">
+        <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B77">
         <v>500</v>
       </c>
       <c r="C77">
+        <v>20</v>
+      </c>
+      <c r="D77">
+        <v>400</v>
+      </c>
+      <c r="E77" t="s">
+        <v>11</v>
+      </c>
+      <c r="F77" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" t="s">
+        <v>5</v>
+      </c>
+      <c r="I77" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>41</v>
+      </c>
+      <c r="B78">
+        <v>500</v>
+      </c>
+      <c r="C78">
         <v>15</v>
       </c>
-      <c r="D77">
+      <c r="D78">
         <v>8000</v>
       </c>
-      <c r="H77" t="s">
+      <c r="H78" t="s">
         <v>7</v>
       </c>
-      <c r="I77" t="s">
+      <c r="I78" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B78" s="8">
+      <c r="B79" s="8">
         <v>500</v>
       </c>
-      <c r="C78" s="8">
+      <c r="C79" s="8">
         <v>30</v>
       </c>
-      <c r="D78" s="8">
+      <c r="D79" s="8">
         <v>16000</v>
       </c>
-      <c r="E78" s="8"/>
-      <c r="F78" s="8"/>
-      <c r="G78" s="8"/>
-      <c r="H78" s="8" t="s">
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I78" s="8" t="s">
+      <c r="I79" s="8" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B79" s="1">
-        <v>550</v>
-      </c>
-      <c r="C79" s="1">
-        <v>25</v>
-      </c>
-      <c r="D79" s="1">
-        <v>6000</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B80" s="1">
         <v>550</v>
@@ -2981,7 +2986,7 @@
         <v>6000</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>7</v>
@@ -2991,12 +2996,12 @@
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B81" s="1">
         <v>550</v>
@@ -3008,22 +3013,22 @@
         <v>6000</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B82" s="1">
         <v>550</v>
@@ -3034,46 +3039,73 @@
       <c r="D82" s="1">
         <v>6000</v>
       </c>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1" t="s">
+      <c r="E82" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F82" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H82" s="1"/>
       <c r="I82" s="1" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B83" s="1">
+        <v>550</v>
+      </c>
+      <c r="C83" s="1">
+        <v>25</v>
+      </c>
+      <c r="D83" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B83" s="8">
+      <c r="B84" s="8">
         <v>600</v>
       </c>
-      <c r="C83" s="8">
+      <c r="C84" s="8">
         <v>30</v>
       </c>
-      <c r="D83" s="8">
+      <c r="D84" s="8">
         <v>16000</v>
       </c>
-      <c r="E83" s="8" t="s">
+      <c r="E84" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F83" s="8" t="s">
+      <c r="F84" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G83" s="8" t="s">
+      <c r="G84" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H83" s="8"/>
-      <c r="I83" s="8" t="s">
+      <c r="H84" s="8"/>
+      <c r="I84" s="8" t="s">
         <v>161</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A43:I83">
-    <sortCondition ref="B42:B83"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A43:I84">
+    <sortCondition ref="B42:B84"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rename Nordic Carved items
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FA9EED-CA96-4AF4-A721-DAA5E8FBB21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E500E9-D354-4FF7-A708-14699D786976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
   <sheets>
     <sheet name="Armors" sheetId="1" r:id="rId1"/>
@@ -230,9 +230,6 @@
     <t>Heavy_Madness</t>
   </si>
   <si>
-    <t>Heavy_NordicCarved</t>
-  </si>
-  <si>
     <t>Heavy_Orcish</t>
   </si>
   <si>
@@ -648,6 +645,9 @@
   </si>
   <si>
     <t>Light_Chainmail</t>
+  </si>
+  <si>
+    <t>Heavy_Quicksilver</t>
   </si>
 </sst>
 </file>
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="P64" sqref="P64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,13 +1105,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" t="s">
         <v>163</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>164</v>
-      </c>
-      <c r="D1" t="s">
-        <v>165</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1126,7 +1126,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1149,12 +1149,12 @@
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3">
         <v>500</v>
@@ -1172,12 +1172,12 @@
         <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4">
         <v>500</v>
@@ -1192,7 +1192,7 @@
         <v>9</v>
       </c>
       <c r="I4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1219,7 +1219,7 @@
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1242,12 +1242,12 @@
         <v>1</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B7" s="3">
         <v>600</v>
@@ -1265,7 +1265,7 @@
         <v>11</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1292,12 +1292,12 @@
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B9" s="3">
         <v>600</v>
@@ -1315,12 +1315,12 @@
         <v>11</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B10" s="3">
         <v>600</v>
@@ -1338,12 +1338,12 @@
         <v>11</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="3">
         <v>600</v>
@@ -1365,12 +1365,12 @@
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B12" s="3">
         <v>600</v>
@@ -1392,12 +1392,12 @@
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="3">
         <v>600</v>
@@ -1415,7 +1415,7 @@
         <v>11</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
         <v>1000</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
         <v>9</v>
@@ -1441,7 +1441,7 @@
         <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1464,7 +1464,7 @@
         <v>11</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1487,7 +1487,7 @@
         <v>11</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1510,7 +1510,7 @@
         <v>11</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1533,12 +1533,12 @@
         <v>11</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B19" s="2">
         <v>700</v>
@@ -1556,12 +1556,12 @@
         <v>11</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B20" s="2">
         <v>700</v>
@@ -1576,15 +1576,15 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B21">
         <v>700</v>
@@ -1596,7 +1596,7 @@
         <v>1500</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
         <v>9</v>
@@ -1605,7 +1605,7 @@
         <v>10</v>
       </c>
       <c r="I21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1628,7 +1628,7 @@
         <v>14</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1651,12 +1651,12 @@
         <v>14</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>63</v>
+        <v>202</v>
       </c>
       <c r="B24" s="5">
         <v>800</v>
@@ -1680,12 +1680,12 @@
         <v>13</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="5">
         <v>800</v>
@@ -1697,7 +1697,7 @@
         <v>1500</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>9</v>
@@ -1707,12 +1707,12 @@
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="5">
         <v>800</v>
@@ -1736,12 +1736,12 @@
         <v>16</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27">
         <v>800</v>
@@ -1756,12 +1756,12 @@
         <v>11</v>
       </c>
       <c r="I27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B28">
         <v>900</v>
@@ -1773,15 +1773,15 @@
         <v>2000</v>
       </c>
       <c r="H28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B29">
         <v>900</v>
@@ -1793,10 +1793,10 @@
         <v>2000</v>
       </c>
       <c r="H29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1813,7 +1813,7 @@
         <v>2000</v>
       </c>
       <c r="E30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F30" t="s">
         <v>9</v>
@@ -1822,12 +1822,12 @@
         <v>5</v>
       </c>
       <c r="I30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B31" s="8">
         <v>900</v>
@@ -1842,10 +1842,10 @@
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1865,10 +1865,10 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1885,7 +1885,7 @@
         <v>10000</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
@@ -1893,12 +1893,12 @@
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B34" s="1">
         <v>1000</v>
@@ -1910,7 +1910,7 @@
         <v>10000</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
@@ -1918,7 +1918,7 @@
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1935,22 +1935,22 @@
         <v>10000</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" s="1">
         <v>1000</v>
@@ -1972,12 +1972,12 @@
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B37" s="1">
         <v>1000</v>
@@ -1992,10 +1992,10 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2012,22 +2012,22 @@
         <v>20000</v>
       </c>
       <c r="E38" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F38" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="8"/>
       <c r="I38" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B39" s="7">
         <v>1200</v>
@@ -2042,15 +2042,15 @@
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B40" s="7">
         <v>1200</v>
@@ -2069,7 +2069,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B41" s="7">
         <v>1200</v>
@@ -2084,10 +2084,10 @@
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2107,7 +2107,7 @@
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2130,12 +2130,12 @@
         <v>5</v>
       </c>
       <c r="I43" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B44" s="4">
         <v>300</v>
@@ -2153,7 +2153,7 @@
         <v>1</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2176,7 +2176,7 @@
         <v>1</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2257,7 +2257,7 @@
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2280,12 +2280,12 @@
         <v>1</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B50" s="4">
         <v>300</v>
@@ -2305,12 +2305,12 @@
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B51" s="4">
         <v>300</v>
@@ -2328,12 +2328,12 @@
         <v>10</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B52" s="4">
         <v>300</v>
@@ -2351,7 +2351,7 @@
         <v>10</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2374,7 +2374,7 @@
         <v>1</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2397,12 +2397,12 @@
         <v>1</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B55" s="4">
         <v>300</v>
@@ -2420,7 +2420,7 @@
         <v>1</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2443,12 +2443,12 @@
         <v>1</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B57" s="4">
         <v>300</v>
@@ -2485,12 +2485,12 @@
         <v>1</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B59" s="4">
         <v>300</v>
@@ -2508,7 +2508,7 @@
         <v>1</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2528,12 +2528,12 @@
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B61">
         <v>300</v>
@@ -2548,7 +2548,7 @@
         <v>1</v>
       </c>
       <c r="I61" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2571,7 +2571,7 @@
         <v>1</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2594,7 +2594,7 @@
         <v>1</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2617,7 +2617,7 @@
         <v>1</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -2637,7 +2637,7 @@
         <v>11</v>
       </c>
       <c r="I65" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -2663,12 +2663,12 @@
         <v>10</v>
       </c>
       <c r="I66" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B67" s="5">
         <v>400</v>
@@ -2686,7 +2686,7 @@
         <v>7</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -2713,12 +2713,12 @@
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B69">
         <v>400</v>
@@ -2742,12 +2742,12 @@
         <v>16</v>
       </c>
       <c r="I69" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B70">
         <v>400</v>
@@ -2759,7 +2759,7 @@
         <v>1000</v>
       </c>
       <c r="E70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F70" t="s">
         <v>1</v>
@@ -2768,7 +2768,7 @@
         <v>5</v>
       </c>
       <c r="I70" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -2788,7 +2788,7 @@
         <v>14</v>
       </c>
       <c r="I71" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -2814,7 +2814,7 @@
         <v>10</v>
       </c>
       <c r="I72" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -2834,7 +2834,7 @@
         <v>11</v>
       </c>
       <c r="I73" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -2854,12 +2854,12 @@
         <v>8</v>
       </c>
       <c r="I74" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B75">
         <v>500</v>
@@ -2871,7 +2871,7 @@
         <v>1000</v>
       </c>
       <c r="E75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F75" t="s">
         <v>1</v>
@@ -2880,7 +2880,7 @@
         <v>5</v>
       </c>
       <c r="I75" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -2900,7 +2900,7 @@
         <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -2926,7 +2926,7 @@
         <v>5</v>
       </c>
       <c r="I77" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -2946,12 +2946,12 @@
         <v>7</v>
       </c>
       <c r="I78" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B79" s="8">
         <v>500</v>
@@ -2969,7 +2969,7 @@
         <v>12</v>
       </c>
       <c r="I79" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -2996,7 +2996,7 @@
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3050,7 +3050,7 @@
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3073,7 +3073,7 @@
         <v>2</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -3100,7 +3100,7 @@
       </c>
       <c r="H84" s="8"/>
       <c r="I84" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3127,18 +3127,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" t="s">
         <v>163</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>164</v>
-      </c>
-      <c r="D1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3">
         <v>-50</v>
@@ -3166,7 +3166,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4">
         <v>-50</v>
@@ -3180,7 +3180,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5">
         <v>-50</v>
@@ -3194,7 +3194,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6">
         <v>-50</v>
@@ -3208,7 +3208,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B7">
         <v>30</v>
@@ -3219,7 +3219,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8">
         <v>25</v>
@@ -3233,7 +3233,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9">
         <v>50</v>
@@ -3247,7 +3247,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10">
         <v>50</v>
@@ -3261,7 +3261,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B11">
         <v>50</v>
@@ -3275,7 +3275,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B12">
         <v>50</v>
@@ -3315,7 +3315,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -3329,7 +3329,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3343,7 +3343,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3357,7 +3357,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -3371,7 +3371,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -3392,7 +3392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B796E76-FF31-432C-A859-43C3EAF890A5}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -3405,32 +3405,32 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" t="s">
         <v>163</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>164</v>
       </c>
-      <c r="E1" t="s">
-        <v>165</v>
-      </c>
       <c r="F1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E3">
         <v>5000</v>
@@ -3441,25 +3441,25 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E7">
         <v>5000</v>
@@ -3470,10 +3470,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" t="s">
         <v>197</v>
-      </c>
-      <c r="B8" t="s">
-        <v>198</v>
       </c>
       <c r="E8">
         <v>5000</v>
@@ -3484,10 +3484,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9">
         <v>50</v>
@@ -3501,70 +3501,70 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E22">
         <v>80000</v>
@@ -3575,30 +3575,30 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C27">
         <v>50</v>
@@ -3612,10 +3612,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D28">
         <v>-4</v>
@@ -3629,50 +3629,50 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E37">
         <v>80000</v>
@@ -3683,15 +3683,15 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C39">
         <v>25</v>
@@ -3705,10 +3705,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E40">
         <v>50000</v>
@@ -3719,10 +3719,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C41">
         <v>50</v>
@@ -3736,15 +3736,15 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E43">
         <v>300</v>
@@ -3755,10 +3755,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B44" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E44">
         <v>5000</v>

</xml_diff>

<commit_message>
Restore chitin heavy armor
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E500E9-D354-4FF7-A708-14699D786976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518AFD58-A9BA-4F32-9128-F23F8953542F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
   <sheets>
     <sheet name="Armors" sheetId="1" r:id="rId1"/>
@@ -152,9 +152,6 @@
     <t>Light_PenitusOculatus</t>
   </si>
   <si>
-    <t>Light_ReinforcedChitin</t>
-  </si>
-  <si>
     <t>Light_Scale</t>
   </si>
   <si>
@@ -648,6 +645,9 @@
   </si>
   <si>
     <t>Heavy_Quicksilver</t>
+  </si>
+  <si>
+    <t>Heavy_Chitin</t>
   </si>
 </sst>
 </file>
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,13 +1105,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" t="s">
         <v>162</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>163</v>
-      </c>
-      <c r="D1" t="s">
-        <v>164</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1126,12 +1126,12 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>202</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -1140,21 +1140,24 @@
         <v>40</v>
       </c>
       <c r="D2">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>500</v>
@@ -1172,12 +1175,12 @@
         <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>193</v>
       </c>
       <c r="B4">
         <v>500</v>
@@ -1188,43 +1191,39 @@
       <c r="D4">
         <v>250</v>
       </c>
-      <c r="H4" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
       <c r="I4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="3">
-        <v>600</v>
-      </c>
-      <c r="C5" s="3">
-        <v>50</v>
-      </c>
-      <c r="D5" s="3">
-        <v>300</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5">
+        <v>500</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>250</v>
+      </c>
+      <c r="H5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3" t="s">
-        <v>161</v>
+      <c r="I5" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B6" s="3">
         <v>600</v>
@@ -1233,21 +1232,25 @@
         <v>50</v>
       </c>
       <c r="D6" s="3">
-        <v>500</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>1</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>187</v>
+        <v>57</v>
       </c>
       <c r="B7" s="3">
         <v>600</v>
@@ -1262,15 +1265,15 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>59</v>
+        <v>186</v>
       </c>
       <c r="B8" s="3">
         <v>600</v>
@@ -1281,23 +1284,19 @@
       <c r="D8" s="3">
         <v>500</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>183</v>
+        <v>58</v>
       </c>
       <c r="B9" s="3">
         <v>600</v>
@@ -1308,19 +1307,23 @@
       <c r="D9" s="3">
         <v>500</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B10" s="3">
         <v>600</v>
@@ -1338,12 +1341,12 @@
         <v>11</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>65</v>
+        <v>188</v>
       </c>
       <c r="B11" s="3">
         <v>600</v>
@@ -1354,23 +1357,19 @@
       <c r="D11" s="3">
         <v>500</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>193</v>
+        <v>64</v>
       </c>
       <c r="B12" s="3">
         <v>600</v>
@@ -1392,12 +1391,12 @@
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>67</v>
+        <v>192</v>
       </c>
       <c r="B13" s="3">
         <v>600</v>
@@ -1408,68 +1407,72 @@
       <c r="D13" s="3">
         <v>500</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3"/>
       <c r="I13" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14">
+      <c r="A14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="3">
         <v>600</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
+        <v>50</v>
+      </c>
+      <c r="D14" s="3">
+        <v>500</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>600</v>
+      </c>
+      <c r="C15">
         <v>40</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>1000</v>
       </c>
-      <c r="E14" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" t="s">
         <v>9</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>10</v>
       </c>
-      <c r="I14" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="2">
-        <v>700</v>
-      </c>
-      <c r="C15" s="2">
-        <v>50</v>
-      </c>
-      <c r="D15" s="2">
-        <v>5000</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>143</v>
+      <c r="I15" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B16" s="2">
         <v>700</v>
@@ -1478,7 +1481,7 @@
         <v>50</v>
       </c>
       <c r="D16" s="2">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1487,12 +1490,12 @@
         <v>11</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B17" s="2">
         <v>700</v>
@@ -1501,7 +1504,7 @@
         <v>50</v>
       </c>
       <c r="D17" s="2">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1510,12 +1513,12 @@
         <v>11</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B18" s="2">
         <v>700</v>
@@ -1533,12 +1536,12 @@
         <v>11</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>184</v>
+        <v>59</v>
       </c>
       <c r="B19" s="2">
         <v>700</v>
@@ -1556,12 +1559,12 @@
         <v>11</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B20" s="2">
         <v>700</v>
@@ -1576,64 +1579,64 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>186</v>
+        <v>11</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>141</v>
-      </c>
-      <c r="B21">
+      <c r="A21" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B21" s="2">
         <v>700</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>50</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22">
+        <v>700</v>
+      </c>
+      <c r="C22">
+        <v>50</v>
+      </c>
+      <c r="D22">
         <v>1500</v>
       </c>
-      <c r="E21" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" t="s">
         <v>9</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G22" t="s">
         <v>10</v>
       </c>
-      <c r="I21" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="5">
-        <v>800</v>
-      </c>
-      <c r="C22" s="5">
-        <v>60</v>
-      </c>
-      <c r="D22" s="5">
-        <v>400</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>143</v>
+      <c r="I22" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B23" s="5">
         <v>800</v>
@@ -1651,12 +1654,12 @@
         <v>14</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>202</v>
+        <v>56</v>
       </c>
       <c r="B24" s="5">
         <v>800</v>
@@ -1665,27 +1668,21 @@
         <v>60</v>
       </c>
       <c r="D24" s="5">
-        <v>1000</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>5</v>
-      </c>
+        <v>400</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
       <c r="H24" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>63</v>
+        <v>201</v>
       </c>
       <c r="B25" s="5">
         <v>800</v>
@@ -1694,25 +1691,27 @@
         <v>60</v>
       </c>
       <c r="D25" s="5">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H25" s="5"/>
+      <c r="H25" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="I25" s="5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B26" s="5">
         <v>800</v>
@@ -1721,62 +1720,69 @@
         <v>60</v>
       </c>
       <c r="D26" s="5">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="5"/>
+      <c r="I26" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="5">
+        <v>800</v>
+      </c>
+      <c r="C27" s="5">
+        <v>60</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1000</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27">
-        <v>800</v>
-      </c>
-      <c r="C27">
-        <v>50</v>
-      </c>
-      <c r="D27">
-        <v>5000</v>
-      </c>
-      <c r="H27" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27" t="s">
-        <v>143</v>
+      <c r="G27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
       <c r="B28">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="C28">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D28">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="H28" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="I28" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1787,21 +1793,21 @@
         <v>900</v>
       </c>
       <c r="C29">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D29">
         <v>2000</v>
       </c>
       <c r="H29" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="I29" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>197</v>
       </c>
       <c r="B30">
         <v>900</v>
@@ -1812,68 +1818,65 @@
       <c r="D30">
         <v>2000</v>
       </c>
-      <c r="E30" t="s">
+      <c r="H30" t="s">
+        <v>69</v>
+      </c>
+      <c r="I30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31">
+        <v>900</v>
+      </c>
+      <c r="C31">
         <v>70</v>
       </c>
-      <c r="F30" t="s">
+      <c r="D31">
+        <v>2000</v>
+      </c>
+      <c r="E31" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" t="s">
         <v>9</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G31" t="s">
         <v>5</v>
       </c>
-      <c r="I30" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="B31" s="8">
+      <c r="I31" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B32" s="8">
         <v>900</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C32" s="8">
         <v>70</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D32" s="8">
         <v>20000</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C32" s="1">
-        <v>80</v>
-      </c>
-      <c r="D32" s="1">
-        <v>20000</v>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>145</v>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B33" s="1">
         <v>1000</v>
@@ -1882,23 +1885,21 @@
         <v>80</v>
       </c>
       <c r="D33" s="1">
-        <v>10000</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>73</v>
-      </c>
+        <v>20000</v>
+      </c>
+      <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="I33" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>192</v>
+        <v>54</v>
       </c>
       <c r="B34" s="1">
         <v>1000</v>
@@ -1910,7 +1911,7 @@
         <v>10000</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
@@ -1918,12 +1919,12 @@
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>62</v>
+        <v>191</v>
       </c>
       <c r="B35" s="1">
         <v>1000</v>
@@ -1935,22 +1936,20 @@
         <v>10000</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>73</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B36" s="1">
         <v>1000</v>
@@ -1962,10 +1961,10 @@
         <v>10000</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>5</v>
@@ -1977,7 +1976,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>180</v>
+        <v>63</v>
       </c>
       <c r="B37" s="1">
         <v>1000</v>
@@ -1988,69 +1987,73 @@
       <c r="D37" s="1">
         <v>10000</v>
       </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="E37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="8">
+      <c r="A38" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B38" s="1">
         <v>1000</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="1">
+        <v>80</v>
+      </c>
+      <c r="D38" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C39" s="8">
         <v>70</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D39" s="8">
         <v>20000</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E39" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F38" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G38" s="8" t="s">
+      <c r="G39" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" s="7">
-        <v>1200</v>
-      </c>
-      <c r="C39" s="7">
-        <v>100</v>
-      </c>
-      <c r="D39" s="7">
-        <v>50000</v>
-      </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>144</v>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>176</v>
+        <v>84</v>
       </c>
       <c r="B40" s="7">
         <v>1200</v>
@@ -2064,12 +2067,16 @@
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
+      <c r="H40" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B41" s="7">
         <v>1200</v>
@@ -2083,36 +2090,35 @@
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
-      <c r="H41" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>144</v>
-      </c>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42">
-        <v>250</v>
-      </c>
-      <c r="C42">
-        <v>8</v>
-      </c>
-      <c r="D42">
+      <c r="A42" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B42" s="7">
+        <v>1200</v>
+      </c>
+      <c r="C42" s="7">
         <v>100</v>
       </c>
-      <c r="H42" t="s">
-        <v>1</v>
-      </c>
-      <c r="I42" t="s">
+      <c r="D42" s="7">
+        <v>50000</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I42" s="7" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B43">
         <v>250</v>
@@ -2123,42 +2129,39 @@
       <c r="D43">
         <v>100</v>
       </c>
-      <c r="E43" t="s">
+      <c r="H43" t="s">
         <v>1</v>
       </c>
-      <c r="G43" t="s">
+      <c r="I43" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44">
+        <v>250</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44">
+        <v>100</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1</v>
+      </c>
+      <c r="G44" t="s">
         <v>5</v>
       </c>
-      <c r="I43" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" s="4">
-        <v>300</v>
-      </c>
-      <c r="C44" s="4">
-        <v>10</v>
-      </c>
-      <c r="D44" s="4">
-        <v>200</v>
-      </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>143</v>
+      <c r="I44" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="B45" s="4">
         <v>300</v>
@@ -2176,12 +2179,12 @@
         <v>1</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B46" s="4">
         <v>300</v>
@@ -2192,23 +2195,19 @@
       <c r="D46" s="4">
         <v>200</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F46" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H46" s="4"/>
       <c r="I46" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B47" s="4">
         <v>300</v>
@@ -2223,19 +2222,19 @@
         <v>1</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B48" s="4">
         <v>300</v>
@@ -2250,19 +2249,19 @@
         <v>1</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B49" s="4">
         <v>300</v>
@@ -2273,19 +2272,23 @@
       <c r="D49" s="4">
         <v>200</v>
       </c>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4" t="s">
+      <c r="E49" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="F49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H49" s="4"/>
       <c r="I49" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>179</v>
+        <v>33</v>
       </c>
       <c r="B50" s="4">
         <v>300</v>
@@ -2294,23 +2297,21 @@
         <v>10</v>
       </c>
       <c r="D50" s="4">
-        <v>400</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="E50" s="4"/>
       <c r="F50" s="4"/>
-      <c r="G50" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="I50" s="4" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="B51" s="4">
         <v>300</v>
@@ -2321,19 +2322,21 @@
       <c r="D51" s="4">
         <v>400</v>
       </c>
-      <c r="E51" s="4"/>
+      <c r="E51" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="G51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H51" s="4"/>
       <c r="I51" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B52" s="4">
         <v>300</v>
@@ -2351,12 +2354,12 @@
         <v>10</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>39</v>
+        <v>190</v>
       </c>
       <c r="B53" s="4">
         <v>300</v>
@@ -2365,21 +2368,21 @@
         <v>10</v>
       </c>
       <c r="D53" s="4">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B54" s="4">
         <v>300</v>
@@ -2388,7 +2391,7 @@
         <v>10</v>
       </c>
       <c r="D54" s="4">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -2397,12 +2400,12 @@
         <v>1</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="B55" s="4">
         <v>300</v>
@@ -2411,7 +2414,7 @@
         <v>10</v>
       </c>
       <c r="D55" s="4">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
@@ -2420,12 +2423,12 @@
         <v>1</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="B56" s="4">
         <v>300</v>
@@ -2443,12 +2446,12 @@
         <v>1</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>177</v>
+        <v>42</v>
       </c>
       <c r="B57" s="4">
         <v>300</v>
@@ -2462,12 +2465,16 @@
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
+      <c r="H57" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>46</v>
+        <v>176</v>
       </c>
       <c r="B58" s="4">
         <v>300</v>
@@ -2481,16 +2488,12 @@
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
-      <c r="H58" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>143</v>
-      </c>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="B59" s="4">
         <v>300</v>
@@ -2508,32 +2511,35 @@
         <v>1</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>29</v>
-      </c>
-      <c r="B60">
+      <c r="A60" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" s="4">
         <v>300</v>
       </c>
-      <c r="C60">
-        <v>15</v>
-      </c>
-      <c r="D60">
-        <v>400</v>
-      </c>
-      <c r="H60" t="s">
+      <c r="C60" s="4">
+        <v>10</v>
+      </c>
+      <c r="D60" s="4">
+        <v>200</v>
+      </c>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I60" t="s">
-        <v>143</v>
+      <c r="I60" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="B61">
         <v>300</v>
@@ -2548,35 +2554,32 @@
         <v>1</v>
       </c>
       <c r="I61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B62" s="6">
-        <v>350</v>
-      </c>
-      <c r="C62" s="6">
-        <v>12</v>
-      </c>
-      <c r="D62" s="6">
+      <c r="A62" t="s">
+        <v>81</v>
+      </c>
+      <c r="B62">
+        <v>300</v>
+      </c>
+      <c r="C62">
+        <v>15</v>
+      </c>
+      <c r="D62">
         <v>400</v>
       </c>
-      <c r="E62" s="6"/>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
-      <c r="H62" s="6" t="s">
+      <c r="H62" t="s">
         <v>1</v>
       </c>
-      <c r="I62" s="6" t="s">
-        <v>143</v>
+      <c r="I62" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B63" s="6">
         <v>350</v>
@@ -2585,7 +2588,7 @@
         <v>12</v>
       </c>
       <c r="D63" s="6">
-        <v>10000</v>
+        <v>400</v>
       </c>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
@@ -2594,12 +2597,12 @@
         <v>1</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B64" s="6">
         <v>350</v>
@@ -2608,7 +2611,7 @@
         <v>12</v>
       </c>
       <c r="D64" s="6">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
@@ -2617,32 +2620,35 @@
         <v>1</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>17</v>
-      </c>
-      <c r="B65">
-        <v>400</v>
-      </c>
-      <c r="C65">
-        <v>20</v>
-      </c>
-      <c r="D65">
-        <v>400</v>
-      </c>
-      <c r="H65" t="s">
-        <v>11</v>
-      </c>
-      <c r="I65" t="s">
-        <v>143</v>
+      <c r="A65" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B65" s="6">
+        <v>350</v>
+      </c>
+      <c r="C65" s="6">
+        <v>12</v>
+      </c>
+      <c r="D65" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B66">
         <v>400</v>
@@ -2651,47 +2657,44 @@
         <v>20</v>
       </c>
       <c r="D66">
+        <v>400</v>
+      </c>
+      <c r="H66" t="s">
+        <v>11</v>
+      </c>
+      <c r="I66" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67">
+        <v>400</v>
+      </c>
+      <c r="C67">
+        <v>20</v>
+      </c>
+      <c r="D67">
         <v>800</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E67" t="s">
         <v>8</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F67" t="s">
         <v>9</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G67" t="s">
         <v>10</v>
       </c>
-      <c r="I66" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="B67" s="5">
-        <v>400</v>
-      </c>
-      <c r="C67" s="5">
-        <v>15</v>
-      </c>
-      <c r="D67" s="5">
-        <v>800</v>
-      </c>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I67" s="5" t="s">
-        <v>149</v>
+      <c r="I67" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>23</v>
+        <v>189</v>
       </c>
       <c r="B68" s="5">
         <v>400</v>
@@ -2702,46 +2705,40 @@
       <c r="D68" s="5">
         <v>800</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="I68" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" s="5">
+        <v>400</v>
+      </c>
+      <c r="C69" s="5">
+        <v>15</v>
+      </c>
+      <c r="D69" s="5">
+        <v>800</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G68" s="5" t="s">
+      <c r="G69" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>201</v>
-      </c>
-      <c r="B69">
-        <v>400</v>
-      </c>
-      <c r="C69">
-        <v>30</v>
-      </c>
-      <c r="D69">
-        <v>600</v>
-      </c>
-      <c r="E69" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" t="s">
-        <v>16</v>
-      </c>
-      <c r="G69" t="s">
-        <v>5</v>
-      </c>
-      <c r="H69" t="s">
-        <v>16</v>
-      </c>
-      <c r="I69" t="s">
+      <c r="H69" s="5"/>
+      <c r="I69" s="5" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2756,65 +2753,68 @@
         <v>30</v>
       </c>
       <c r="D70">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="E70" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="F70" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G70" t="s">
         <v>5</v>
       </c>
+      <c r="H70" t="s">
+        <v>16</v>
+      </c>
       <c r="I70" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>25</v>
+        <v>199</v>
       </c>
       <c r="B71">
         <v>400</v>
       </c>
       <c r="C71">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D71">
-        <v>100</v>
-      </c>
-      <c r="H71" t="s">
-        <v>14</v>
+        <v>1000</v>
+      </c>
+      <c r="E71" t="s">
+        <v>69</v>
+      </c>
+      <c r="F71" t="s">
+        <v>1</v>
+      </c>
+      <c r="G71" t="s">
+        <v>5</v>
       </c>
       <c r="I71" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B72">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="C72">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D72">
-        <v>1000</v>
-      </c>
-      <c r="E72" t="s">
-        <v>8</v>
-      </c>
-      <c r="F72" t="s">
-        <v>9</v>
-      </c>
-      <c r="G72" t="s">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="H72" t="s">
+        <v>14</v>
       </c>
       <c r="I72" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -2834,7 +2834,7 @@
         <v>11</v>
       </c>
       <c r="I73" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -2854,12 +2854,12 @@
         <v>8</v>
       </c>
       <c r="I74" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B75">
         <v>500</v>
@@ -2871,7 +2871,7 @@
         <v>1000</v>
       </c>
       <c r="E75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F75" t="s">
         <v>1</v>
@@ -2880,7 +2880,7 @@
         <v>5</v>
       </c>
       <c r="I75" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -2900,12 +2900,12 @@
         <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B77">
         <v>500</v>
@@ -2926,12 +2926,12 @@
         <v>5</v>
       </c>
       <c r="I77" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B78">
         <v>500</v>
@@ -2946,12 +2946,12 @@
         <v>7</v>
       </c>
       <c r="I78" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B79" s="8">
         <v>500</v>
@@ -2969,7 +2969,7 @@
         <v>12</v>
       </c>
       <c r="I79" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -2996,7 +2996,7 @@
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3023,12 +3023,12 @@
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B82" s="1">
         <v>550</v>
@@ -3050,12 +3050,12 @@
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B83" s="1">
         <v>550</v>
@@ -3073,7 +3073,7 @@
         <v>2</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -3100,12 +3100,12 @@
       </c>
       <c r="H84" s="8"/>
       <c r="I84" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A43:I84">
-    <sortCondition ref="B42:B84"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A44:I84">
+    <sortCondition ref="B43:B84"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3127,18 +3127,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" t="s">
         <v>162</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>163</v>
-      </c>
-      <c r="D1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3">
         <v>-50</v>
@@ -3166,7 +3166,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4">
         <v>-50</v>
@@ -3180,7 +3180,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5">
         <v>-50</v>
@@ -3194,7 +3194,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6">
         <v>-50</v>
@@ -3208,7 +3208,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B7">
         <v>30</v>
@@ -3219,7 +3219,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8">
         <v>25</v>
@@ -3233,7 +3233,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9">
         <v>50</v>
@@ -3247,7 +3247,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10">
         <v>50</v>
@@ -3261,7 +3261,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B11">
         <v>50</v>
@@ -3275,7 +3275,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B12">
         <v>50</v>
@@ -3315,7 +3315,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -3329,7 +3329,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3343,7 +3343,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3357,7 +3357,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -3371,7 +3371,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -3392,7 +3392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B796E76-FF31-432C-A859-43C3EAF890A5}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -3405,32 +3405,32 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" t="s">
         <v>162</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>163</v>
       </c>
-      <c r="E1" t="s">
-        <v>164</v>
-      </c>
       <c r="F1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E3">
         <v>5000</v>
@@ -3441,25 +3441,25 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E7">
         <v>5000</v>
@@ -3470,10 +3470,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B8" t="s">
         <v>196</v>
-      </c>
-      <c r="B8" t="s">
-        <v>197</v>
       </c>
       <c r="E8">
         <v>5000</v>
@@ -3484,10 +3484,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9">
         <v>50</v>
@@ -3501,70 +3501,70 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E22">
         <v>80000</v>
@@ -3575,30 +3575,30 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C27">
         <v>50</v>
@@ -3612,10 +3612,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D28">
         <v>-4</v>
@@ -3629,50 +3629,50 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E37">
         <v>80000</v>
@@ -3683,15 +3683,15 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C39">
         <v>25</v>
@@ -3705,10 +3705,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E40">
         <v>50000</v>
@@ -3719,10 +3719,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C41">
         <v>50</v>
@@ -3736,15 +3736,15 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E43">
         <v>300</v>
@@ -3755,10 +3755,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E44">
         <v>5000</v>

</xml_diff>

<commit_message>
Disable content from Netch Leather Armor DLC
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272C5DCF-F575-48F2-A785-FE0C1FDA56F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A831569E-8B52-4A67-A946-09BE8A6686CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="202">
   <si>
     <t>Amber</t>
   </si>
@@ -642,6 +642,9 @@
   </si>
   <si>
     <t>Heavy_Chitin</t>
+  </si>
+  <si>
+    <t>Charcoal</t>
   </si>
 </sst>
 </file>
@@ -1090,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="J75" sqref="J75"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2352,12 +2355,16 @@
       <c r="D52" s="4">
         <v>400</v>
       </c>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4" t="s">
+      <c r="E52" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="F52" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H52" s="4"/>
       <c r="I52" s="4" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Armor bonus for Vigilant armors
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A831569E-8B52-4A67-A946-09BE8A6686CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F89D08-9530-4E6E-BE74-54D4EB481293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="199">
   <si>
     <t>Amber</t>
   </si>
@@ -590,9 +590,6 @@
     <t>Heavy_Tyranus</t>
   </si>
   <si>
-    <t>Silver</t>
-  </si>
-  <si>
     <t>Heavy_Halvar</t>
   </si>
   <si>
@@ -608,15 +605,6 @@
     <t>Light_ShadowedNetchLeather</t>
   </si>
   <si>
-    <t>Heavy_EbonySpellKnight</t>
-  </si>
-  <si>
-    <t>Heavy_SteelSpellKnight</t>
-  </si>
-  <si>
-    <t>Heavy_IronSpellKnight</t>
-  </si>
-  <si>
     <t>Light_PaintedNetchLeather</t>
   </si>
   <si>
@@ -645,6 +633,9 @@
   </si>
   <si>
     <t>Charcoal</t>
+  </si>
+  <si>
+    <t>Heavy_Carcette</t>
   </si>
 </sst>
 </file>
@@ -1091,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,7 +1127,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -1185,7 +1176,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>66</v>
       </c>
       <c r="B4">
         <v>500</v>
@@ -1196,39 +1187,43 @@
       <c r="D4">
         <v>250</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="3">
+        <v>600</v>
+      </c>
+      <c r="C5" s="3">
+        <v>50</v>
+      </c>
+      <c r="D5" s="3">
+        <v>300</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5">
-        <v>500</v>
-      </c>
-      <c r="C5">
-        <v>40</v>
-      </c>
-      <c r="D5">
-        <v>250</v>
-      </c>
-      <c r="H5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" t="s">
-        <v>140</v>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B6" s="3">
         <v>600</v>
@@ -1237,25 +1232,21 @@
         <v>50</v>
       </c>
       <c r="D6" s="3">
-        <v>300</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="3"/>
+        <v>500</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="I6" s="3" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>56</v>
+        <v>183</v>
       </c>
       <c r="B7" s="3">
         <v>600</v>
@@ -1270,7 +1261,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>140</v>
@@ -1278,7 +1269,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>184</v>
+        <v>57</v>
       </c>
       <c r="B8" s="3">
         <v>600</v>
@@ -1289,19 +1280,23 @@
       <c r="D8" s="3">
         <v>500</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>57</v>
+        <v>180</v>
       </c>
       <c r="B9" s="3">
         <v>600</v>
@@ -1312,23 +1307,19 @@
       <c r="D9" s="3">
         <v>500</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B10" s="3">
         <v>600</v>
@@ -1351,7 +1342,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>186</v>
+        <v>63</v>
       </c>
       <c r="B11" s="3">
         <v>600</v>
@@ -1362,19 +1353,23 @@
       <c r="D11" s="3">
         <v>500</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B12" s="3">
         <v>600</v>
@@ -1385,99 +1380,91 @@
       <c r="D12" s="3">
         <v>500</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="I12" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13">
+        <v>600</v>
+      </c>
+      <c r="C13">
+        <v>40</v>
+      </c>
+      <c r="D13">
+        <v>1000</v>
+      </c>
+      <c r="E13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B13" s="3">
-        <v>600</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2">
+        <v>700</v>
+      </c>
+      <c r="C14" s="2">
         <v>50</v>
       </c>
-      <c r="D13" s="3">
-        <v>500</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="D14" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="3">
-        <v>600</v>
-      </c>
-      <c r="C14" s="3">
+      <c r="I14" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2">
+        <v>700</v>
+      </c>
+      <c r="C15" s="2">
         <v>50</v>
       </c>
-      <c r="D14" s="3">
-        <v>500</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3" t="s">
+      <c r="D15" s="2">
+        <v>2500</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15">
-        <v>600</v>
-      </c>
-      <c r="C15">
-        <v>40</v>
-      </c>
-      <c r="D15">
-        <v>1000</v>
-      </c>
-      <c r="E15" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" t="s">
-        <v>155</v>
+      <c r="I15" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B16" s="2">
         <v>700</v>
@@ -1486,7 +1473,7 @@
         <v>50</v>
       </c>
       <c r="D16" s="2">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1500,7 +1487,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B17" s="2">
         <v>700</v>
@@ -1509,7 +1496,7 @@
         <v>50</v>
       </c>
       <c r="D17" s="2">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1523,7 +1510,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>181</v>
       </c>
       <c r="B18" s="2">
         <v>700</v>
@@ -1545,103 +1532,107 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="2">
+      <c r="A19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19">
         <v>700</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19">
         <v>50</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19">
+        <v>1500</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="5">
+        <v>800</v>
+      </c>
+      <c r="C20" s="5">
+        <v>60</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1500</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="5">
+        <v>800</v>
+      </c>
+      <c r="C21" s="5">
+        <v>60</v>
+      </c>
+      <c r="D21" s="5">
         <v>1000</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2" t="s">
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B20" s="2">
-        <v>700</v>
-      </c>
-      <c r="C20" s="2">
-        <v>50</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1000</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B21" s="2">
-        <v>700</v>
-      </c>
-      <c r="C21" s="2">
-        <v>50</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1000</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" s="5" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>138</v>
-      </c>
-      <c r="B22">
-        <v>700</v>
-      </c>
-      <c r="C22">
-        <v>50</v>
-      </c>
-      <c r="D22">
+      <c r="A22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="5">
+        <v>800</v>
+      </c>
+      <c r="C22" s="5">
+        <v>60</v>
+      </c>
+      <c r="D22" s="5">
         <v>1500</v>
       </c>
-      <c r="E22" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G22" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" t="s">
-        <v>154</v>
+      <c r="G22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>195</v>
+        <v>54</v>
       </c>
       <c r="B23" s="5">
         <v>800</v>
@@ -1650,21 +1641,21 @@
         <v>60</v>
       </c>
       <c r="D23" s="5">
-        <v>1500</v>
+        <v>400</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B24" s="5">
         <v>800</v>
@@ -1673,25 +1664,21 @@
         <v>60</v>
       </c>
       <c r="D24" s="5">
-        <v>1500</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H24" s="5"/>
+        <v>400</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="I24" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>54</v>
+        <v>195</v>
       </c>
       <c r="B25" s="5">
         <v>800</v>
@@ -1700,21 +1687,27 @@
         <v>60</v>
       </c>
       <c r="D25" s="5">
-        <v>400</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+        <v>1000</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="H25" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B26" s="5">
         <v>800</v>
@@ -1723,21 +1716,27 @@
         <v>60</v>
       </c>
       <c r="D26" s="5">
-        <v>400</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+        <v>1000</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="H26" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B27" s="5">
         <v>800</v>
@@ -1748,77 +1747,68 @@
       <c r="D27" s="5">
         <v>1000</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
       <c r="H27" s="5" t="s">
-        <v>13</v>
+        <v>161</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="5">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28">
         <v>800</v>
       </c>
-      <c r="C28" s="5">
-        <v>60</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1000</v>
-      </c>
-      <c r="E28" s="5" t="s">
+      <c r="C28">
+        <v>50</v>
+      </c>
+      <c r="D28">
+        <v>5000</v>
+      </c>
+      <c r="H28" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>144</v>
+      <c r="I28" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B29">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="C29">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D29">
-        <v>5000</v>
-      </c>
-      <c r="H29" t="s">
-        <v>11</v>
+        <v>2000</v>
+      </c>
+      <c r="E29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" t="s">
+        <v>5</v>
       </c>
       <c r="I29" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>192</v>
       </c>
       <c r="B30">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="C30">
         <v>60</v>
@@ -1826,65 +1816,64 @@
       <c r="D30">
         <v>2000</v>
       </c>
-      <c r="E30" t="s">
+      <c r="H30" t="s">
         <v>73</v>
-      </c>
-      <c r="F30" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" t="s">
-        <v>5</v>
       </c>
       <c r="I30" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>196</v>
-      </c>
-      <c r="B31">
+      <c r="A31" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B31" s="8">
+        <v>900</v>
+      </c>
+      <c r="C31" s="8">
+        <v>70</v>
+      </c>
+      <c r="D31" s="8">
+        <v>20000</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="1">
         <v>1000</v>
       </c>
-      <c r="C31">
-        <v>60</v>
-      </c>
-      <c r="D31">
-        <v>2000</v>
-      </c>
-      <c r="H31" t="s">
-        <v>73</v>
-      </c>
-      <c r="I31" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B32" s="8">
-        <v>900</v>
-      </c>
-      <c r="C32" s="8">
-        <v>70</v>
-      </c>
-      <c r="D32" s="8">
-        <v>20000</v>
-      </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>156</v>
+      <c r="C32" s="1">
+        <v>80</v>
+      </c>
+      <c r="D32" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1">
         <v>1000</v>
@@ -1896,20 +1885,22 @@
         <v>10000</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>189</v>
+        <v>62</v>
       </c>
       <c r="B34" s="1">
         <v>1000</v>
@@ -1921,20 +1912,22 @@
         <v>10000</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F34" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="G34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="B35" s="1">
         <v>1000</v>
@@ -1945,100 +1938,88 @@
       <c r="D35" s="1">
         <v>10000</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F35" s="1" t="s">
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="I35" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C36" s="8">
+        <v>70</v>
+      </c>
+      <c r="D36" s="8">
+        <v>20000</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C36" s="1">
-        <v>80</v>
-      </c>
-      <c r="D36" s="1">
-        <v>10000</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1" t="s">
-        <v>150</v>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B37" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C37" s="1">
-        <v>80</v>
-      </c>
-      <c r="D37" s="1">
-        <v>10000</v>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
+      <c r="A37" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="7">
+        <v>1200</v>
+      </c>
+      <c r="C37" s="7">
+        <v>100</v>
+      </c>
+      <c r="D37" s="7">
+        <v>50000</v>
+      </c>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="I37" s="1" t="s">
-        <v>143</v>
+      <c r="I37" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="8">
-        <v>1000</v>
-      </c>
-      <c r="C38" s="8">
-        <v>70</v>
-      </c>
-      <c r="D38" s="8">
-        <v>20000</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8" t="s">
-        <v>156</v>
-      </c>
+      <c r="A38" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B38" s="7">
+        <v>1200</v>
+      </c>
+      <c r="C38" s="7">
+        <v>100</v>
+      </c>
+      <c r="D38" s="7">
+        <v>50000</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>83</v>
+        <v>179</v>
       </c>
       <c r="B39" s="7">
         <v>1200</v>
@@ -2060,93 +2041,97 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B40" s="7">
-        <v>1200</v>
-      </c>
-      <c r="C40" s="7">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>250</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
         <v>100</v>
       </c>
-      <c r="D40" s="7">
-        <v>50000</v>
-      </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
+      <c r="H40" t="s">
+        <v>1</v>
+      </c>
+      <c r="I40" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="B41" s="7">
-        <v>1200</v>
-      </c>
-      <c r="C41" s="7">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41">
+        <v>250</v>
+      </c>
+      <c r="C41">
+        <v>8</v>
+      </c>
+      <c r="D41">
         <v>100</v>
       </c>
-      <c r="D41" s="7">
-        <v>50000</v>
-      </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>141</v>
+      <c r="E41" t="s">
+        <v>1</v>
+      </c>
+      <c r="G41" t="s">
+        <v>5</v>
+      </c>
+      <c r="I41" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42">
-        <v>250</v>
-      </c>
-      <c r="C42">
-        <v>8</v>
-      </c>
-      <c r="D42">
-        <v>100</v>
-      </c>
-      <c r="H42" t="s">
+      <c r="A42" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="4">
+        <v>300</v>
+      </c>
+      <c r="C42" s="4">
+        <v>10</v>
+      </c>
+      <c r="D42" s="4">
+        <v>200</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43">
-        <v>250</v>
-      </c>
-      <c r="C43">
-        <v>8</v>
-      </c>
-      <c r="D43">
-        <v>100</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="A43" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="4">
+        <v>300</v>
+      </c>
+      <c r="C43" s="4">
+        <v>10</v>
+      </c>
+      <c r="D43" s="4">
+        <v>200</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G43" t="s">
-        <v>5</v>
-      </c>
-      <c r="I43" t="s">
+      <c r="I43" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="B44" s="4">
         <v>300</v>
@@ -2157,19 +2142,23 @@
       <c r="D44" s="4">
         <v>200</v>
       </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4" t="s">
+      <c r="E44" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="F44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44" s="4"/>
       <c r="I44" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B45" s="4">
         <v>300</v>
@@ -2180,19 +2169,23 @@
       <c r="D45" s="4">
         <v>200</v>
       </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4" t="s">
+      <c r="E45" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="F45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H45" s="4"/>
       <c r="I45" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B46" s="4">
         <v>300</v>
@@ -2219,7 +2212,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B47" s="4">
         <v>300</v>
@@ -2230,23 +2223,19 @@
       <c r="D47" s="4">
         <v>200</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H47" s="4"/>
       <c r="I47" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>32</v>
+        <v>176</v>
       </c>
       <c r="B48" s="4">
         <v>300</v>
@@ -2255,25 +2244,23 @@
         <v>10</v>
       </c>
       <c r="D48" s="4">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F48" s="4"/>
       <c r="G48" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>33</v>
+        <v>188</v>
       </c>
       <c r="B49" s="4">
         <v>300</v>
@@ -2282,21 +2269,21 @@
         <v>10</v>
       </c>
       <c r="D49" s="4">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="B50" s="4">
         <v>300</v>
@@ -2310,7 +2297,9 @@
       <c r="E50" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F50" s="4"/>
+      <c r="F50" s="4" t="s">
+        <v>197</v>
+      </c>
       <c r="G50" s="4" t="s">
         <v>5</v>
       </c>
@@ -2321,7 +2310,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>192</v>
+        <v>38</v>
       </c>
       <c r="B51" s="4">
         <v>300</v>
@@ -2330,21 +2319,21 @@
         <v>10</v>
       </c>
       <c r="D51" s="4">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>188</v>
+        <v>39</v>
       </c>
       <c r="B52" s="4">
         <v>300</v>
@@ -2355,23 +2344,19 @@
       <c r="D52" s="4">
         <v>400</v>
       </c>
-      <c r="E52" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="I52" s="4" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="B53" s="4">
         <v>300</v>
@@ -2394,7 +2379,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B54" s="4">
         <v>300</v>
@@ -2403,7 +2388,7 @@
         <v>10</v>
       </c>
       <c r="D54" s="4">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -2417,7 +2402,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="B55" s="4">
         <v>300</v>
@@ -2431,16 +2416,12 @@
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
-      <c r="H55" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>140</v>
-      </c>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B56" s="4">
         <v>300</v>
@@ -2463,7 +2444,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>174</v>
+        <v>82</v>
       </c>
       <c r="B57" s="4">
         <v>300</v>
@@ -2477,98 +2458,102 @@
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
+      <c r="H57" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B58" s="4">
+      <c r="A58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58">
         <v>300</v>
       </c>
-      <c r="C58" s="4">
-        <v>10</v>
-      </c>
-      <c r="D58" s="4">
-        <v>200</v>
-      </c>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4" t="s">
+      <c r="C58">
+        <v>15</v>
+      </c>
+      <c r="D58">
+        <v>400</v>
+      </c>
+      <c r="H58" t="s">
         <v>1</v>
       </c>
-      <c r="I58" s="4" t="s">
+      <c r="I58" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" s="4">
+      <c r="A59" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59">
         <v>300</v>
       </c>
-      <c r="C59" s="4">
-        <v>10</v>
-      </c>
-      <c r="D59" s="4">
-        <v>200</v>
-      </c>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4" t="s">
+      <c r="C59">
+        <v>15</v>
+      </c>
+      <c r="D59">
+        <v>400</v>
+      </c>
+      <c r="H59" t="s">
         <v>1</v>
       </c>
-      <c r="I59" s="4" t="s">
+      <c r="I59" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>29</v>
-      </c>
-      <c r="B60">
-        <v>300</v>
-      </c>
-      <c r="C60">
-        <v>15</v>
-      </c>
-      <c r="D60">
+      <c r="A60" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="6">
+        <v>350</v>
+      </c>
+      <c r="C60" s="6">
+        <v>12</v>
+      </c>
+      <c r="D60" s="6">
         <v>400</v>
       </c>
-      <c r="H60" t="s">
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I60" s="6" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>80</v>
-      </c>
-      <c r="B61">
-        <v>300</v>
-      </c>
-      <c r="C61">
-        <v>15</v>
-      </c>
-      <c r="D61">
-        <v>400</v>
-      </c>
-      <c r="H61" t="s">
+      <c r="A61" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="6">
+        <v>350</v>
+      </c>
+      <c r="C61" s="6">
+        <v>12</v>
+      </c>
+      <c r="D61" s="6">
+        <v>10000</v>
+      </c>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I61" t="s">
-        <v>140</v>
+      <c r="I61" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B62" s="6">
         <v>350</v>
@@ -2577,7 +2562,7 @@
         <v>12</v>
       </c>
       <c r="D62" s="6">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
@@ -2591,7 +2576,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B63" s="6">
         <v>350</v>
@@ -2600,7 +2585,7 @@
         <v>12</v>
       </c>
       <c r="D63" s="6">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
@@ -2609,84 +2594,84 @@
         <v>1</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B64" s="6">
+      <c r="A64" t="s">
+        <v>37</v>
+      </c>
+      <c r="B64">
         <v>350</v>
       </c>
-      <c r="C64" s="6">
-        <v>12</v>
-      </c>
-      <c r="D64" s="6">
-        <v>600</v>
-      </c>
-      <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
-      <c r="G64" s="6"/>
-      <c r="H64" s="6" t="s">
+      <c r="C64">
+        <v>15</v>
+      </c>
+      <c r="D64">
+        <v>400</v>
+      </c>
+      <c r="E64" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" t="s">
         <v>1</v>
       </c>
-      <c r="I64" s="6" t="s">
-        <v>140</v>
+      <c r="G64" t="s">
+        <v>5</v>
+      </c>
+      <c r="I64" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B65" s="6">
-        <v>350</v>
-      </c>
-      <c r="C65" s="6">
-        <v>12</v>
-      </c>
-      <c r="D65" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E65" s="6"/>
-      <c r="F65" s="6"/>
-      <c r="G65" s="6"/>
-      <c r="H65" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I65" s="6" t="s">
-        <v>140</v>
+      <c r="A65" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B65" s="5">
+        <v>400</v>
+      </c>
+      <c r="C65" s="5">
+        <v>20</v>
+      </c>
+      <c r="D65" s="5">
+        <v>800</v>
+      </c>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>37</v>
-      </c>
-      <c r="B66">
-        <v>350</v>
-      </c>
-      <c r="C66">
-        <v>15</v>
-      </c>
-      <c r="D66">
+      <c r="A66" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B66" s="5">
         <v>400</v>
       </c>
-      <c r="E66" t="s">
+      <c r="C66" s="5">
+        <v>20</v>
+      </c>
+      <c r="D66" s="5">
+        <v>400</v>
+      </c>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F66" t="s">
-        <v>1</v>
-      </c>
-      <c r="G66" t="s">
-        <v>5</v>
-      </c>
-      <c r="I66" t="s">
-        <v>145</v>
+      <c r="I66" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>187</v>
+        <v>20</v>
       </c>
       <c r="B67" s="5">
         <v>400</v>
@@ -2697,19 +2682,23 @@
       <c r="D67" s="5">
         <v>800</v>
       </c>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="E67" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H67" s="5"/>
       <c r="I67" s="5" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B68" s="5">
         <v>400</v>
@@ -2718,13 +2707,13 @@
         <v>20</v>
       </c>
       <c r="D68" s="5">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
       <c r="H68" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>140</v>
@@ -2732,7 +2721,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B69" s="5">
         <v>400</v>
@@ -2744,22 +2733,22 @@
         <v>800</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H69" s="5"/>
       <c r="I69" s="5" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B70" s="5">
         <v>400</v>
@@ -2768,219 +2757,223 @@
         <v>20</v>
       </c>
       <c r="D70" s="5">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
       <c r="H70" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B71" s="5">
+      <c r="A71" t="s">
+        <v>194</v>
+      </c>
+      <c r="B71">
         <v>400</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C71">
+        <v>30</v>
+      </c>
+      <c r="D71">
+        <v>600</v>
+      </c>
+      <c r="E71" t="s">
+        <v>11</v>
+      </c>
+      <c r="F71" t="s">
+        <v>16</v>
+      </c>
+      <c r="G71" t="s">
+        <v>5</v>
+      </c>
+      <c r="H71" t="s">
+        <v>16</v>
+      </c>
+      <c r="I71" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>193</v>
+      </c>
+      <c r="B72">
+        <v>400</v>
+      </c>
+      <c r="C72">
+        <v>30</v>
+      </c>
+      <c r="D72">
+        <v>1000</v>
+      </c>
+      <c r="E72" t="s">
+        <v>68</v>
+      </c>
+      <c r="F72" t="s">
+        <v>1</v>
+      </c>
+      <c r="G72" t="s">
+        <v>5</v>
+      </c>
+      <c r="I72" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B73" s="9">
+        <v>500</v>
+      </c>
+      <c r="C73" s="9">
+        <v>30</v>
+      </c>
+      <c r="D73" s="9">
+        <v>600</v>
+      </c>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B74" s="9">
+        <v>500</v>
+      </c>
+      <c r="C74" s="9">
+        <v>30</v>
+      </c>
+      <c r="D74" s="9">
+        <v>1000</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H74" s="9"/>
+      <c r="I74" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>40</v>
+      </c>
+      <c r="B75">
+        <v>500</v>
+      </c>
+      <c r="C75">
         <v>20</v>
       </c>
-      <c r="D71" s="5">
-        <v>800</v>
-      </c>
-      <c r="E71" s="5" t="s">
+      <c r="D75">
+        <v>5000</v>
+      </c>
+      <c r="H75" t="s">
         <v>7</v>
       </c>
-      <c r="F71" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G71" s="5" t="s">
+      <c r="I75" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B76" s="8">
+        <v>500</v>
+      </c>
+      <c r="C76" s="8">
+        <v>30</v>
+      </c>
+      <c r="D76" s="8">
+        <v>16000</v>
+      </c>
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I76" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B77" s="1">
+        <v>550</v>
+      </c>
+      <c r="C77" s="1">
+        <v>25</v>
+      </c>
+      <c r="D77" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B72" s="5">
-        <v>400</v>
-      </c>
-      <c r="C72" s="5">
-        <v>20</v>
-      </c>
-      <c r="D72" s="5">
-        <v>5000</v>
-      </c>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I72" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>198</v>
-      </c>
-      <c r="B73">
-        <v>400</v>
-      </c>
-      <c r="C73">
-        <v>30</v>
-      </c>
-      <c r="D73">
-        <v>600</v>
-      </c>
-      <c r="E73" t="s">
-        <v>11</v>
-      </c>
-      <c r="F73" t="s">
-        <v>16</v>
-      </c>
-      <c r="G73" t="s">
+      <c r="H77" s="1"/>
+      <c r="I77" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B78" s="1">
+        <v>550</v>
+      </c>
+      <c r="C78" s="1">
+        <v>25</v>
+      </c>
+      <c r="D78" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G78" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H73" t="s">
-        <v>16</v>
-      </c>
-      <c r="I73" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>197</v>
-      </c>
-      <c r="B74">
-        <v>400</v>
-      </c>
-      <c r="C74">
-        <v>30</v>
-      </c>
-      <c r="D74">
-        <v>1000</v>
-      </c>
-      <c r="E74" t="s">
-        <v>68</v>
-      </c>
-      <c r="F74" t="s">
-        <v>1</v>
-      </c>
-      <c r="G74" t="s">
-        <v>5</v>
-      </c>
-      <c r="I74" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B75" s="9">
-        <v>500</v>
-      </c>
-      <c r="C75" s="9">
-        <v>30</v>
-      </c>
-      <c r="D75" s="9">
-        <v>600</v>
-      </c>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I75" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="B76" s="9">
-        <v>500</v>
-      </c>
-      <c r="C76" s="9">
-        <v>30</v>
-      </c>
-      <c r="D76" s="9">
-        <v>1000</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F76" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G76" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H76" s="9"/>
-      <c r="I76" s="9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>40</v>
-      </c>
-      <c r="B77">
-        <v>500</v>
-      </c>
-      <c r="C77">
-        <v>20</v>
-      </c>
-      <c r="D77">
-        <v>5000</v>
-      </c>
-      <c r="H77" t="s">
-        <v>7</v>
-      </c>
-      <c r="I77" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="B78" s="8">
-        <v>500</v>
-      </c>
-      <c r="C78" s="8">
-        <v>30</v>
-      </c>
-      <c r="D78" s="8">
-        <v>16000</v>
-      </c>
-      <c r="E78" s="8"/>
-      <c r="F78" s="8"/>
-      <c r="G78" s="8"/>
-      <c r="H78" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I78" s="8" t="s">
-        <v>157</v>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B79" s="1">
         <v>550</v>
@@ -2992,22 +2985,22 @@
         <v>6000</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B80" s="1">
         <v>550</v>
@@ -3018,100 +3011,46 @@
       <c r="D80" s="1">
         <v>6000</v>
       </c>
-      <c r="E80" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G80" s="1" t="s">
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B81" s="8">
+        <v>600</v>
+      </c>
+      <c r="C81" s="8">
+        <v>30</v>
+      </c>
+      <c r="D81" s="8">
+        <v>16000</v>
+      </c>
+      <c r="E81" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B81" s="1">
-        <v>550</v>
-      </c>
-      <c r="C81" s="1">
-        <v>25</v>
-      </c>
-      <c r="D81" s="1">
-        <v>6000</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B82" s="1">
-        <v>550</v>
-      </c>
-      <c r="C82" s="1">
-        <v>25</v>
-      </c>
-      <c r="D82" s="1">
-        <v>6000</v>
-      </c>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I82" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B83" s="8">
-        <v>600</v>
-      </c>
-      <c r="C83" s="8">
-        <v>30</v>
-      </c>
-      <c r="D83" s="8">
-        <v>16000</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G83" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H83" s="8"/>
-      <c r="I83" s="8" t="s">
+      <c r="H81" s="8"/>
+      <c r="I81" s="8" t="s">
         <v>157</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A43:I83">
-    <sortCondition ref="B42:B83"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:I81">
+    <sortCondition ref="B40:B81"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3476,10 +3415,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B8" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E8">
         <v>5000</v>

</xml_diff>

<commit_message>
Armor bonus for Blades armor
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34C1C58-0087-4113-8685-DC0E18CAD88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DDA2AB-21F8-4FBE-9BF1-C6608F927036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
@@ -185,9 +185,6 @@
     <t>Heavy_AncientNord</t>
   </si>
   <si>
-    <t>Heavy_Blades</t>
-  </si>
-  <si>
     <t>Heavy_Bonemold</t>
   </si>
   <si>
@@ -642,6 +639,9 @@
   </si>
   <si>
     <t>Heavy_HaldynQuicksilver</t>
+  </si>
+  <si>
+    <t>Heavy_Akaviri</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1091,7 @@
   <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,13 +1107,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" t="s">
         <v>159</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>160</v>
-      </c>
-      <c r="D1" t="s">
-        <v>161</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1128,12 +1128,12 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -1154,12 +1154,12 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B3" s="4">
         <v>500</v>
@@ -1177,12 +1177,12 @@
         <v>9</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="4">
         <v>500</v>
@@ -1202,12 +1202,12 @@
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="4">
         <v>500</v>
@@ -1225,7 +1225,7 @@
         <v>9</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1252,12 +1252,12 @@
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="3">
         <v>600</v>
@@ -1275,12 +1275,12 @@
         <v>1</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B8" s="3">
         <v>600</v>
@@ -1298,12 +1298,12 @@
         <v>11</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="3">
         <v>600</v>
@@ -1325,12 +1325,12 @@
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B10" s="3">
         <v>600</v>
@@ -1348,12 +1348,12 @@
         <v>11</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B11" s="3">
         <v>600</v>
@@ -1371,12 +1371,12 @@
         <v>11</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="3">
         <v>600</v>
@@ -1398,12 +1398,12 @@
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="3">
         <v>600</v>
@@ -1421,12 +1421,12 @@
         <v>11</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14">
         <v>600</v>
@@ -1438,7 +1438,7 @@
         <v>1000</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F14" t="s">
         <v>9</v>
@@ -1447,7 +1447,7 @@
         <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1470,12 +1470,12 @@
         <v>11</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>200</v>
       </c>
       <c r="B16" s="2">
         <v>700</v>
@@ -1493,12 +1493,12 @@
         <v>11</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="2">
         <v>700</v>
@@ -1516,12 +1516,12 @@
         <v>11</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2">
         <v>700</v>
@@ -1539,12 +1539,12 @@
         <v>11</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B19" s="2">
         <v>700</v>
@@ -1562,12 +1562,12 @@
         <v>11</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B20">
         <v>700</v>
@@ -1579,7 +1579,7 @@
         <v>1500</v>
       </c>
       <c r="E20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F20" t="s">
         <v>9</v>
@@ -1588,12 +1588,12 @@
         <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B21" s="5">
         <v>800</v>
@@ -1608,15 +1608,15 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B22" s="5">
         <v>800</v>
@@ -1634,12 +1634,12 @@
         <v>13</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B23" s="5">
         <v>800</v>
@@ -1657,12 +1657,12 @@
         <v>11</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" s="5">
         <v>800</v>
@@ -1674,7 +1674,7 @@
         <v>1500</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>9</v>
@@ -1684,12 +1684,12 @@
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="5">
         <v>800</v>
@@ -1707,12 +1707,12 @@
         <v>14</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="5">
         <v>800</v>
@@ -1730,12 +1730,12 @@
         <v>14</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B27" s="5">
         <v>800</v>
@@ -1759,12 +1759,12 @@
         <v>13</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="5">
         <v>800</v>
@@ -1788,12 +1788,12 @@
         <v>16</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B29" s="5">
         <v>800</v>
@@ -1808,15 +1808,15 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30">
         <v>800</v>
@@ -1831,12 +1831,12 @@
         <v>11</v>
       </c>
       <c r="I30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31">
         <v>900</v>
@@ -1848,7 +1848,7 @@
         <v>2000</v>
       </c>
       <c r="E31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F31" t="s">
         <v>9</v>
@@ -1857,12 +1857,12 @@
         <v>5</v>
       </c>
       <c r="I31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B32">
         <v>1000</v>
@@ -1874,15 +1874,15 @@
         <v>2000</v>
       </c>
       <c r="H32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B33" s="8">
         <v>900</v>
@@ -1897,15 +1897,15 @@
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" s="1">
         <v>1000</v>
@@ -1917,7 +1917,7 @@
         <v>10000</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
@@ -1925,12 +1925,12 @@
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="1">
         <v>1000</v>
@@ -1942,22 +1942,22 @@
         <v>10000</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B36" s="1">
         <v>1000</v>
@@ -1979,12 +1979,12 @@
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B37" s="1">
         <v>1000</v>
@@ -1999,15 +1999,15 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38" s="8">
         <v>1000</v>
@@ -2019,22 +2019,22 @@
         <v>20000</v>
       </c>
       <c r="E38" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F38" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="8"/>
       <c r="I38" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B39" s="7">
         <v>1200</v>
@@ -2049,15 +2049,15 @@
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B40" s="7">
         <v>1200</v>
@@ -2076,7 +2076,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B41" s="7">
         <v>1200</v>
@@ -2091,10 +2091,10 @@
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2114,7 +2114,7 @@
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2137,12 +2137,12 @@
         <v>5</v>
       </c>
       <c r="I43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" s="4">
         <v>300</v>
@@ -2160,7 +2160,7 @@
         <v>1</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2183,7 +2183,7 @@
         <v>1</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2237,7 +2237,7 @@
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2264,7 +2264,7 @@
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2287,12 +2287,12 @@
         <v>1</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B50" s="4">
         <v>300</v>
@@ -2312,12 +2312,12 @@
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B51" s="4">
         <v>300</v>
@@ -2335,12 +2335,12 @@
         <v>10</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B52" s="4">
         <v>300</v>
@@ -2355,14 +2355,14 @@
         <v>10</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H52" s="4"/>
       <c r="I52" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2385,7 +2385,7 @@
         <v>1</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2408,12 +2408,12 @@
         <v>1</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B55" s="4">
         <v>300</v>
@@ -2431,7 +2431,7 @@
         <v>1</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2454,12 +2454,12 @@
         <v>1</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B57" s="4">
         <v>300</v>
@@ -2496,12 +2496,12 @@
         <v>1</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B59" s="4">
         <v>300</v>
@@ -2519,7 +2519,7 @@
         <v>1</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2539,12 +2539,12 @@
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B61">
         <v>300</v>
@@ -2559,7 +2559,7 @@
         <v>1</v>
       </c>
       <c r="I61" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2582,7 +2582,7 @@
         <v>1</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2605,7 +2605,7 @@
         <v>1</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2628,7 +2628,7 @@
         <v>1</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -2651,7 +2651,7 @@
         <v>1</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -2677,12 +2677,12 @@
         <v>5</v>
       </c>
       <c r="I66" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B67" s="5">
         <v>400</v>
@@ -2700,7 +2700,7 @@
         <v>7</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -2723,7 +2723,7 @@
         <v>11</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -2750,7 +2750,7 @@
       </c>
       <c r="H69" s="5"/>
       <c r="I69" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -2773,7 +2773,7 @@
         <v>14</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -2800,7 +2800,7 @@
       </c>
       <c r="H71" s="5"/>
       <c r="I71" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -2823,12 +2823,12 @@
         <v>8</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B73">
         <v>400</v>
@@ -2852,12 +2852,12 @@
         <v>16</v>
       </c>
       <c r="I73" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B74">
         <v>400</v>
@@ -2869,7 +2869,7 @@
         <v>1000</v>
       </c>
       <c r="E74" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F74" t="s">
         <v>1</v>
@@ -2878,7 +2878,7 @@
         <v>5</v>
       </c>
       <c r="I74" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -2901,12 +2901,12 @@
         <v>11</v>
       </c>
       <c r="I75" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B76" s="9">
         <v>500</v>
@@ -2918,7 +2918,7 @@
         <v>1000</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F76" s="9" t="s">
         <v>1</v>
@@ -2928,7 +2928,7 @@
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -2948,12 +2948,12 @@
         <v>7</v>
       </c>
       <c r="I77" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B78" s="8">
         <v>500</v>
@@ -2971,7 +2971,7 @@
         <v>12</v>
       </c>
       <c r="I78" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -2998,7 +2998,7 @@
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3052,7 +3052,7 @@
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3075,7 +3075,7 @@
         <v>2</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3102,7 +3102,7 @@
       </c>
       <c r="H83" s="8"/>
       <c r="I83" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -3129,18 +3129,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" t="s">
         <v>159</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>160</v>
-      </c>
-      <c r="D1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -3154,7 +3154,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3">
         <v>-50</v>
@@ -3168,7 +3168,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B4">
         <v>-50</v>
@@ -3182,7 +3182,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B5">
         <v>-50</v>
@@ -3196,7 +3196,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B6">
         <v>-50</v>
@@ -3210,7 +3210,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7">
         <v>30</v>
@@ -3221,7 +3221,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B8">
         <v>25</v>
@@ -3235,7 +3235,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9">
         <v>50</v>
@@ -3249,7 +3249,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B10">
         <v>50</v>
@@ -3263,7 +3263,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11">
         <v>50</v>
@@ -3277,7 +3277,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B12">
         <v>50</v>
@@ -3317,7 +3317,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -3331,7 +3331,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3345,7 +3345,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3359,7 +3359,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -3373,7 +3373,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -3407,32 +3407,32 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" t="s">
         <v>159</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>160</v>
       </c>
-      <c r="E1" t="s">
-        <v>161</v>
-      </c>
       <c r="F1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3">
         <v>5000</v>
@@ -3443,25 +3443,25 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E7">
         <v>5000</v>
@@ -3472,10 +3472,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" t="s">
         <v>189</v>
-      </c>
-      <c r="B8" t="s">
-        <v>190</v>
       </c>
       <c r="E8">
         <v>5000</v>
@@ -3486,10 +3486,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9">
         <v>50</v>
@@ -3503,70 +3503,70 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E22">
         <v>80000</v>
@@ -3577,30 +3577,30 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C27">
         <v>50</v>
@@ -3614,10 +3614,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D28">
         <v>-4</v>
@@ -3631,50 +3631,50 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E37">
         <v>80000</v>
@@ -3685,15 +3685,15 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C39">
         <v>25</v>
@@ -3707,10 +3707,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E40">
         <v>50000</v>
@@ -3721,10 +3721,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C41">
         <v>50</v>
@@ -3738,15 +3738,15 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E43">
         <v>300</v>
@@ -3757,10 +3757,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E44">
         <v>5000</v>

</xml_diff>

<commit_message>
Finishing Touches - Around the Fire
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DDA2AB-21F8-4FBE-9BF1-C6608F927036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF734F4-85DD-4566-87BA-1CC1071EB902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="201">
   <si>
     <t>Amber</t>
   </si>
@@ -1090,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1747,17 +1747,15 @@
         <v>1000</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H27" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="H27" s="5"/>
       <c r="I27" s="5" t="s">
         <v>143</v>
       </c>
@@ -1971,9 +1969,7 @@
       <c r="E36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
         <v>5</v>
       </c>
@@ -2871,9 +2867,6 @@
       <c r="E74" t="s">
         <v>67</v>
       </c>
-      <c r="F74" t="s">
-        <v>1</v>
-      </c>
       <c r="G74" t="s">
         <v>5</v>
       </c>
@@ -2920,9 +2913,7 @@
       <c r="E76" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F76" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="F76" s="9"/>
       <c r="G76" s="9" t="s">
         <v>5</v>
       </c>
@@ -3044,9 +3035,7 @@
       <c r="E81" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Look up crafting components by full name
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF734F4-85DD-4566-87BA-1CC1071EB902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF220D12-7E07-45A0-AAEF-78FC1F6C6CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
@@ -39,10 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="201">
-  <si>
-    <t>Amber</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="202">
   <si>
     <t>Leather</t>
   </si>
@@ -62,36 +59,15 @@
     <t>Temper</t>
   </si>
   <si>
-    <t>Moonstone</t>
-  </si>
-  <si>
     <t>Chitin Plate</t>
   </si>
   <si>
-    <t>Iron</t>
-  </si>
-  <si>
     <t>Netch Leather</t>
   </si>
   <si>
-    <t>Steel</t>
-  </si>
-  <si>
-    <t>Dragon Scale</t>
-  </si>
-  <si>
-    <t>Quicksilver</t>
-  </si>
-  <si>
     <t>Chaurus Chitin</t>
   </si>
   <si>
-    <t>Malachite</t>
-  </si>
-  <si>
-    <t>Corundum</t>
-  </si>
-  <si>
     <t>Light_Alikr</t>
   </si>
   <si>
@@ -242,24 +218,12 @@
     <t>Heavy_Wolf</t>
   </si>
   <si>
-    <t>Dwarven</t>
-  </si>
-  <si>
     <t>Bone Meal</t>
   </si>
   <si>
     <t>Dragon Bone</t>
   </si>
   <si>
-    <t>Ebony</t>
-  </si>
-  <si>
-    <t>Madness</t>
-  </si>
-  <si>
-    <t>Orichalcum</t>
-  </si>
-  <si>
     <t>Body</t>
   </si>
   <si>
@@ -642,6 +606,45 @@
   </si>
   <si>
     <t>Heavy_Akaviri</t>
+  </si>
+  <si>
+    <t>Dragon Scales</t>
+  </si>
+  <si>
+    <t>Iron Ingot</t>
+  </si>
+  <si>
+    <t>Steel Ingot</t>
+  </si>
+  <si>
+    <t>Quicksilver Ingot</t>
+  </si>
+  <si>
+    <t>Corundum Ingot</t>
+  </si>
+  <si>
+    <t>Gold Ingot</t>
+  </si>
+  <si>
+    <t>Orichalcum Ingot</t>
+  </si>
+  <si>
+    <t>Ebony Ingot</t>
+  </si>
+  <si>
+    <t>Madness Ingot</t>
+  </si>
+  <si>
+    <t>Dwarven Metal Ingot</t>
+  </si>
+  <si>
+    <t>Refined Moonstone</t>
+  </si>
+  <si>
+    <t>Refined Malachite</t>
+  </si>
+  <si>
+    <t>Refined Amber</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1094,7 @@
   <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,33 +1110,33 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D1" t="s">
-        <v>160</v>
+        <v>194</v>
       </c>
       <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -1145,21 +1148,21 @@
         <v>1000</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="B3" s="4">
         <v>500</v>
@@ -1174,15 +1177,15 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B4" s="4">
         <v>500</v>
@@ -1194,20 +1197,20 @@
         <v>250</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B5" s="4">
         <v>500</v>
@@ -1222,15 +1225,15 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B6" s="3">
         <v>600</v>
@@ -1242,22 +1245,22 @@
         <v>300</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3">
         <v>600</v>
@@ -1272,15 +1275,15 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="B8" s="3">
         <v>600</v>
@@ -1295,15 +1298,15 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B9" s="3">
         <v>600</v>
@@ -1315,22 +1318,22 @@
         <v>500</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="B10" s="3">
         <v>600</v>
@@ -1345,15 +1348,15 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="B11" s="3">
         <v>600</v>
@@ -1368,15 +1371,15 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B12" s="3">
         <v>600</v>
@@ -1388,22 +1391,22 @@
         <v>500</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B13" s="3">
         <v>600</v>
@@ -1418,15 +1421,15 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>600</v>
@@ -1438,21 +1441,21 @@
         <v>1000</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I14" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B15" s="2">
         <v>700</v>
@@ -1467,15 +1470,15 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B16" s="2">
         <v>700</v>
@@ -1490,15 +1493,15 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B17" s="2">
         <v>700</v>
@@ -1513,15 +1516,15 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B18" s="2">
         <v>700</v>
@@ -1536,15 +1539,15 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B19" s="2">
         <v>700</v>
@@ -1559,15 +1562,15 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B20">
         <v>700</v>
@@ -1579,21 +1582,21 @@
         <v>1500</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I20" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="B21" s="5">
         <v>800</v>
@@ -1608,15 +1611,15 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5" t="s">
-        <v>67</v>
+        <v>198</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="B22" s="5">
         <v>800</v>
@@ -1631,15 +1634,15 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5" t="s">
-        <v>13</v>
+        <v>192</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="B23" s="5">
         <v>800</v>
@@ -1654,15 +1657,15 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B24" s="5">
         <v>800</v>
@@ -1674,22 +1677,22 @@
         <v>1500</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>67</v>
+        <v>198</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B25" s="5">
         <v>800</v>
@@ -1704,15 +1707,15 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B26" s="5">
         <v>800</v>
@@ -1727,15 +1730,15 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B27" s="5">
         <v>800</v>
@@ -1747,22 +1750,22 @@
         <v>1000</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>13</v>
+        <v>192</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B28" s="5">
         <v>800</v>
@@ -1774,24 +1777,24 @@
         <v>1000</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>16</v>
+        <v>193</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>16</v>
+        <v>193</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B29" s="5">
         <v>800</v>
@@ -1806,15 +1809,15 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5" t="s">
-        <v>160</v>
+        <v>194</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B30">
         <v>800</v>
@@ -1826,15 +1829,15 @@
         <v>5000</v>
       </c>
       <c r="H30" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="I30" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B31">
         <v>900</v>
@@ -1846,21 +1849,21 @@
         <v>2000</v>
       </c>
       <c r="E31" t="s">
-        <v>72</v>
+        <v>195</v>
       </c>
       <c r="F31" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I31" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="B32">
         <v>1000</v>
@@ -1872,15 +1875,15 @@
         <v>2000</v>
       </c>
       <c r="H32" t="s">
-        <v>72</v>
+        <v>195</v>
       </c>
       <c r="I32" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B33" s="8">
         <v>900</v>
@@ -1895,15 +1898,15 @@
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B34" s="1">
         <v>1000</v>
@@ -1915,20 +1918,20 @@
         <v>10000</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>70</v>
+        <v>196</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B35" s="1">
         <v>1000</v>
@@ -1940,22 +1943,22 @@
         <v>10000</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>71</v>
+        <v>197</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>70</v>
+        <v>196</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B36" s="1">
         <v>1000</v>
@@ -1967,20 +1970,20 @@
         <v>10000</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="B37" s="1">
         <v>1000</v>
@@ -1995,15 +1998,15 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>70</v>
+        <v>196</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B38" s="8">
         <v>1000</v>
@@ -2015,22 +2018,22 @@
         <v>20000</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>70</v>
+        <v>196</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H38" s="8"/>
       <c r="I38" s="8" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B39" s="7">
         <v>1200</v>
@@ -2045,15 +2048,15 @@
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7" t="s">
-        <v>70</v>
+        <v>196</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="B40" s="7">
         <v>1200</v>
@@ -2072,7 +2075,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="B41" s="7">
         <v>1200</v>
@@ -2087,15 +2090,15 @@
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7" t="s">
-        <v>70</v>
+        <v>196</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B42">
         <v>250</v>
@@ -2107,15 +2110,15 @@
         <v>100</v>
       </c>
       <c r="H42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B43">
         <v>250</v>
@@ -2127,18 +2130,18 @@
         <v>100</v>
       </c>
       <c r="E43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I43" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B44" s="4">
         <v>300</v>
@@ -2153,15 +2156,15 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B45" s="4">
         <v>300</v>
@@ -2176,15 +2179,15 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B46" s="4">
         <v>300</v>
@@ -2196,22 +2199,22 @@
         <v>200</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B47" s="4">
         <v>300</v>
@@ -2223,22 +2226,22 @@
         <v>200</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B48" s="4">
         <v>300</v>
@@ -2250,22 +2253,22 @@
         <v>200</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B49" s="4">
         <v>300</v>
@@ -2280,15 +2283,15 @@
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B50" s="4">
         <v>300</v>
@@ -2300,20 +2303,20 @@
         <v>400</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B51" s="4">
         <v>300</v>
@@ -2328,15 +2331,15 @@
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B52" s="4">
         <v>300</v>
@@ -2348,22 +2351,22 @@
         <v>400</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H52" s="4"/>
       <c r="I52" s="4" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B53" s="4">
         <v>300</v>
@@ -2378,15 +2381,15 @@
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B54" s="4">
         <v>300</v>
@@ -2401,15 +2404,15 @@
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B55" s="4">
         <v>300</v>
@@ -2424,15 +2427,15 @@
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B56" s="4">
         <v>300</v>
@@ -2447,15 +2450,15 @@
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="B57" s="4">
         <v>300</v>
@@ -2474,7 +2477,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B58" s="4">
         <v>300</v>
@@ -2489,15 +2492,15 @@
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B59" s="4">
         <v>300</v>
@@ -2512,15 +2515,15 @@
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B60">
         <v>300</v>
@@ -2532,15 +2535,15 @@
         <v>400</v>
       </c>
       <c r="H60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B61">
         <v>300</v>
@@ -2552,15 +2555,15 @@
         <v>400</v>
       </c>
       <c r="H61" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B62" s="6">
         <v>350</v>
@@ -2575,15 +2578,15 @@
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
       <c r="H62" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B63" s="6">
         <v>350</v>
@@ -2598,15 +2601,15 @@
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
       <c r="H63" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B64" s="6">
         <v>350</v>
@@ -2621,15 +2624,15 @@
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
       <c r="H64" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B65" s="6">
         <v>350</v>
@@ -2644,15 +2647,15 @@
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
       <c r="H65" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B66">
         <v>350</v>
@@ -2664,21 +2667,21 @@
         <v>400</v>
       </c>
       <c r="E66" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="F66" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I66" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="B67" s="5">
         <v>400</v>
@@ -2693,15 +2696,15 @@
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
       <c r="H67" s="5" t="s">
-        <v>7</v>
+        <v>199</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B68" s="5">
         <v>400</v>
@@ -2716,15 +2719,15 @@
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
       <c r="H68" s="5" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B69" s="5">
         <v>400</v>
@@ -2736,22 +2739,22 @@
         <v>800</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H69" s="5"/>
       <c r="I69" s="5" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B70" s="5">
         <v>400</v>
@@ -2766,15 +2769,15 @@
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
       <c r="H70" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B71" s="5">
         <v>400</v>
@@ -2786,22 +2789,22 @@
         <v>800</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>7</v>
+        <v>199</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>13</v>
+        <v>192</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H71" s="5"/>
       <c r="I71" s="5" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B72" s="5">
         <v>400</v>
@@ -2816,15 +2819,15 @@
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
       <c r="H72" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="B73">
         <v>400</v>
@@ -2836,24 +2839,24 @@
         <v>600</v>
       </c>
       <c r="E73" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="F73" t="s">
-        <v>16</v>
+        <v>193</v>
       </c>
       <c r="G73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H73" t="s">
-        <v>16</v>
+        <v>193</v>
       </c>
       <c r="I73" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="B74">
         <v>400</v>
@@ -2865,18 +2868,18 @@
         <v>1000</v>
       </c>
       <c r="E74" t="s">
-        <v>67</v>
+        <v>198</v>
       </c>
       <c r="G74" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I74" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B75" s="9">
         <v>500</v>
@@ -2891,15 +2894,15 @@
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
       <c r="H75" s="9" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="I75" s="9" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="B76" s="9">
         <v>500</v>
@@ -2911,20 +2914,20 @@
         <v>1000</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>72</v>
+        <v>195</v>
       </c>
       <c r="F76" s="9"/>
       <c r="G76" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="9" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B77">
         <v>500</v>
@@ -2936,15 +2939,15 @@
         <v>5000</v>
       </c>
       <c r="H77" t="s">
-        <v>7</v>
+        <v>199</v>
       </c>
       <c r="I77" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B78" s="8">
         <v>500</v>
@@ -2959,15 +2962,15 @@
       <c r="F78" s="8"/>
       <c r="G78" s="8"/>
       <c r="H78" s="8" t="s">
-        <v>12</v>
+        <v>189</v>
       </c>
       <c r="I78" s="8" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B79" s="1">
         <v>550</v>
@@ -2979,22 +2982,22 @@
         <v>6000</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>7</v>
+        <v>199</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B80" s="1">
         <v>550</v>
@@ -3006,22 +3009,22 @@
         <v>6000</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>15</v>
+        <v>200</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>7</v>
+        <v>199</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B81" s="1">
         <v>550</v>
@@ -3033,20 +3036,20 @@
         <v>6000</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B82" s="1">
         <v>550</v>
@@ -3061,15 +3064,15 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B83" s="8">
         <v>600</v>
@@ -3081,17 +3084,17 @@
         <v>16000</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>12</v>
+        <v>189</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H83" s="8"/>
       <c r="I83" s="8" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3118,18 +3121,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D1" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -3143,7 +3146,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B3">
         <v>-50</v>
@@ -3157,7 +3160,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B4">
         <v>-50</v>
@@ -3171,7 +3174,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B5">
         <v>-50</v>
@@ -3185,7 +3188,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="B6">
         <v>-50</v>
@@ -3199,7 +3202,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="B7">
         <v>30</v>
@@ -3210,7 +3213,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B8">
         <v>25</v>
@@ -3224,7 +3227,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="B9">
         <v>50</v>
@@ -3238,7 +3241,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B10">
         <v>50</v>
@@ -3252,7 +3255,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B11">
         <v>50</v>
@@ -3266,7 +3269,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="B12">
         <v>50</v>
@@ -3295,18 +3298,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -3320,7 +3323,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3334,7 +3337,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3348,7 +3351,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -3362,7 +3365,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -3396,32 +3399,32 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C1" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="D1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="E1" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="F1" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E3">
         <v>5000</v>
@@ -3432,25 +3435,25 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="E7">
         <v>5000</v>
@@ -3461,10 +3464,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="E8">
         <v>5000</v>
@@ -3475,10 +3478,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C9">
         <v>50</v>
@@ -3492,70 +3495,70 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="E22">
         <v>80000</v>
@@ -3566,30 +3569,30 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C27">
         <v>50</v>
@@ -3603,10 +3606,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="D28">
         <v>-4</v>
@@ -3620,50 +3623,50 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E37">
         <v>80000</v>
@@ -3674,15 +3677,15 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C39">
         <v>25</v>
@@ -3696,10 +3699,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="E40">
         <v>50000</v>
@@ -3710,10 +3713,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B41" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C41">
         <v>50</v>
@@ -3727,15 +3730,15 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B43" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="E43">
         <v>300</v>
@@ -3746,10 +3749,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E44">
         <v>5000</v>

</xml_diff>

<commit_message>
Fix column name "Gold"
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF220D12-7E07-45A0-AAEF-78FC1F6C6CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711F60EF-C905-45CA-A862-14FA342DE8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
@@ -1093,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,7 +1116,7 @@
         <v>147</v>
       </c>
       <c r="D1" t="s">
-        <v>194</v>
+        <v>148</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
More flexible patch extension
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711F60EF-C905-45CA-A862-14FA342DE8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579FB0EC-96DA-4B9A-A471-2C1453AA12BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
   <sheets>
     <sheet name="Armors" sheetId="1" r:id="rId1"/>
     <sheet name="Extras" sheetId="5" r:id="rId2"/>
     <sheet name="CraftingQuantities" sheetId="2" r:id="rId3"/>
     <sheet name="Artifacts" sheetId="3" r:id="rId4"/>
+    <sheet name="Patches" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="235">
   <si>
     <t>Leather</t>
   </si>
@@ -645,13 +646,112 @@
   </si>
   <si>
     <t>Refined Amber</t>
+  </si>
+  <si>
+    <t>Heavy_Runic</t>
+  </si>
+  <si>
+    <t>Heavy_DivineWrath</t>
+  </si>
+  <si>
+    <t>Light_Mail</t>
+  </si>
+  <si>
+    <t>Heavy_Hoth</t>
+  </si>
+  <si>
+    <t>Light_NordicScale</t>
+  </si>
+  <si>
+    <t>Heavy_ImperialLoyalist</t>
+  </si>
+  <si>
+    <t>Heavy_NordHero</t>
+  </si>
+  <si>
+    <t>Heavy_Pathfinder</t>
+  </si>
+  <si>
+    <t>Heavy_SoulRipper</t>
+  </si>
+  <si>
+    <t>Heavy_WanderingKnight</t>
+  </si>
+  <si>
+    <t>Light_RogueThief</t>
+  </si>
+  <si>
+    <t>Light_ShadowWarlock</t>
+  </si>
+  <si>
+    <t>Heavy_BlackthornFamily</t>
+  </si>
+  <si>
+    <t>Witchplate Armor Set﻿</t>
+  </si>
+  <si>
+    <t>Lost Paladins of the Divines Wrath Armor</t>
+  </si>
+  <si>
+    <t>Common Clothes and Armors</t>
+  </si>
+  <si>
+    <t>Hoth</t>
+  </si>
+  <si>
+    <t>Scale Nord Armor﻿</t>
+  </si>
+  <si>
+    <t>Talos Housecarl Armor Pack﻿</t>
+  </si>
+  <si>
+    <t>Warmonger Armory</t>
+  </si>
+  <si>
+    <t>Rough Leather Armor</t>
+  </si>
+  <si>
+    <t>Light_RoughLeather</t>
+  </si>
+  <si>
+    <t>Ulag's Legacy</t>
+  </si>
+  <si>
+    <t>Heavy_Blooded</t>
+  </si>
+  <si>
+    <t>Light_Apotheus</t>
+  </si>
+  <si>
+    <t>Light_Duskward</t>
+  </si>
+  <si>
+    <t>Light_Venomfang</t>
+  </si>
+  <si>
+    <t>Heavy_Brunwulf</t>
+  </si>
+  <si>
+    <t>Light_SandAssassin</t>
+  </si>
+  <si>
+    <t>Light_Redguard</t>
+  </si>
+  <si>
+    <t>Inconsequential NPCs</t>
+  </si>
+  <si>
+    <t>Heavy_ForeignEnvoy</t>
+  </si>
+  <si>
+    <t>Light_TownCrier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -669,6 +769,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -743,7 +851,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -755,8 +863,9 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
@@ -767,8 +876,9 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="9"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="10"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="11"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
     <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
     <cellStyle name="60% - Accent3" xfId="3" builtinId="40"/>
@@ -779,6 +889,7 @@
     <cellStyle name="Accent1" xfId="7" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="9" builtinId="41"/>
     <cellStyle name="Accent6" xfId="10" builtinId="49"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1083,7 +1194,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1093,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3291,7 +3402,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3386,7 +3497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B796E76-FF31-432C-A859-43C3EAF890A5}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3764,4 +3875,302 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE05CA9-7B7C-41E3-B17F-147A14B5FFC4}">
+  <dimension ref="A1:E34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>207</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>225</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="E18">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>226</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>100</v>
+      </c>
+      <c r="E19">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>227</v>
+      </c>
+      <c r="B20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
+      </c>
+      <c r="E20">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>209</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>210</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>211</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>212</v>
+      </c>
+      <c r="B26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>230</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>213</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>214</v>
+      </c>
+      <c r="B29" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B30" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>231</v>
+      </c>
+      <c r="B31" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>228</v>
+      </c>
+      <c r="B32" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>202</v>
+      </c>
+      <c r="B34" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A33" r:id="rId1" display="https://www.nexusmods.com/skyrimspecialedition/mods/17053" xr:uid="{51B5E46E-7465-47AA-AFA4-969F70EFB983}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://www.nexusmods.com/skyrim/mods/24253" xr:uid="{8A70CD2B-9C90-40DD-92FE-BFB1B4D4AAA8}"/>
+    <hyperlink ref="A2" r:id="rId3" display="https://www.nexusmods.com/skyrimspecialedition/mods/21305" xr:uid="{864662CC-01F5-469A-A082-72D9FAFD26E1}"/>
+    <hyperlink ref="A4" r:id="rId4" display="https://www.nexusmods.com/skyrimspecialedition/mods/16137" xr:uid="{662CD418-C443-4166-BCEA-C6092D8DC225}"/>
+    <hyperlink ref="A13" r:id="rId5" display="https://www.nexusmods.com/skyrimspecialedition/mods/41118" xr:uid="{4F4C3161-11CF-4A28-9DEA-B51D9BFFF136}"/>
+    <hyperlink ref="A15" r:id="rId6" display="https://www.nexusmods.com/skyrimspecialedition/mods/5540" xr:uid="{0C9D126E-6044-43BA-BC70-95F490971E19}"/>
+    <hyperlink ref="A21" r:id="rId7" display="https://www.nexusmods.com/skyrimspecialedition/mods/17809" xr:uid="{6D47B761-511E-4AF5-89B8-03523BD006E8}"/>
+    <hyperlink ref="A11" r:id="rId8" display="https://www.nexusmods.com/skyrimspecialedition/mods/23725" xr:uid="{57891D5A-6225-4B73-965D-B06155CF14AA}"/>
+    <hyperlink ref="A17" r:id="rId9" display="https://www.nexusmods.com/skyrimspecialedition/mods/20510" xr:uid="{C7690EE7-478C-4CFF-8267-F16EDAAEA3B4}"/>
+    <hyperlink ref="A6" r:id="rId10" display="https://www.nexusmods.com/skyrim/mods/36334" xr:uid="{13EF6B90-3044-4B50-9A34-879079EC938C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Integrate with scripting suite
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CC2C40-E9C0-42D7-8AFF-D136077D818C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EFD851-44D4-41AF-8F0E-167F6A4564D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="236">
   <si>
     <t>Leather</t>
   </si>
@@ -1207,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,9 +1273,6 @@
       <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
-        <v>6</v>
-      </c>
       <c r="J2" t="s">
         <v>142</v>
       </c>
@@ -1602,9 +1599,6 @@
       <c r="G14" t="s">
         <v>7</v>
       </c>
-      <c r="I14" t="s">
-        <v>59</v>
-      </c>
       <c r="J14" t="s">
         <v>142</v>
       </c>
@@ -1761,9 +1755,6 @@
       <c r="G20" t="s">
         <v>7</v>
       </c>
-      <c r="I20" t="s">
-        <v>59</v>
-      </c>
       <c r="J20" t="s">
         <v>141</v>
       </c>
@@ -1895,9 +1886,7 @@
       <c r="H25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="I25" s="5"/>
       <c r="J25" s="5" t="s">
         <v>127</v>
       </c>
@@ -1921,9 +1910,7 @@
       <c r="H26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I26" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="I26" s="5"/>
       <c r="J26" s="5" t="s">
         <v>127</v>
       </c>
@@ -2110,9 +2097,7 @@
       <c r="H33" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I33" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="I33" s="8"/>
       <c r="J33" s="8" t="s">
         <v>143</v>
       </c>
@@ -2254,9 +2239,7 @@
         <v>4</v>
       </c>
       <c r="H38" s="8"/>
-      <c r="I38" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="I38" s="8"/>
       <c r="J38" s="8" t="s">
         <v>143</v>
       </c>
@@ -3062,9 +3045,7 @@
         <v>7</v>
       </c>
       <c r="H69" s="5"/>
-      <c r="I69" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="I69" s="5"/>
       <c r="J69" s="5" t="s">
         <v>142</v>
       </c>
@@ -3088,9 +3069,7 @@
       <c r="H70" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I70" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="I70" s="5"/>
       <c r="J70" s="5" t="s">
         <v>127</v>
       </c>
@@ -3144,9 +3123,7 @@
       <c r="H72" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I72" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="I72" s="5"/>
       <c r="J72" s="5" t="s">
         <v>127</v>
       </c>
@@ -3305,9 +3282,7 @@
       <c r="H78" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="I78" s="8" t="s">
-        <v>189</v>
-      </c>
+      <c r="I78" s="8"/>
       <c r="J78" s="8" t="s">
         <v>144</v>
       </c>
@@ -3451,9 +3426,7 @@
         <v>4</v>
       </c>
       <c r="H83" s="8"/>
-      <c r="I83" s="8" t="s">
-        <v>189</v>
-      </c>
+      <c r="I83" s="8"/>
       <c r="J83" s="8" t="s">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
Heavy Falmer armor has a proper EditorID.
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AB0978-C9A2-46B7-92F3-6FCCE8505017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111BB998-3095-4E9D-B8B8-AB920115D713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
   <sheets>
     <sheet name="Armors" sheetId="1" r:id="rId1"/>
@@ -180,9 +180,6 @@
     <t>Heavy_FalmerHardened</t>
   </si>
   <si>
-    <t>Heavy_FalmerHeavy</t>
-  </si>
-  <si>
     <t>Heavy_Guard</t>
   </si>
   <si>
@@ -766,6 +763,9 @@
   </si>
   <si>
     <t>Light_Fur_Body_KiltWithMantle</t>
+  </si>
+  <si>
+    <t>Heavy_Falmer</t>
   </si>
 </sst>
 </file>
@@ -1233,8 +1233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,13 +1250,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" t="s">
         <v>146</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>147</v>
-      </c>
-      <c r="D1" t="s">
-        <v>148</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1271,18 +1271,18 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -1297,21 +1297,21 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
       </c>
       <c r="J2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3" s="4">
         <v>500</v>
@@ -1326,21 +1326,21 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="4">
         <v>500</v>
@@ -1352,7 +1352,7 @@
         <v>250</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
@@ -1360,18 +1360,18 @@
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="4">
         <v>500</v>
@@ -1386,16 +1386,16 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1412,28 +1412,28 @@
         <v>300</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="3">
         <v>600</v>
@@ -1454,15 +1454,15 @@
         <v>0</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8" s="3">
         <v>600</v>
@@ -1477,21 +1477,21 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="3">
         <v>600</v>
@@ -1503,28 +1503,28 @@
         <v>500</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B10" s="3">
         <v>600</v>
@@ -1539,21 +1539,21 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B11" s="3">
         <v>600</v>
@@ -1568,21 +1568,21 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="3">
         <v>600</v>
@@ -1594,28 +1594,28 @@
         <v>500</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" s="3">
         <v>600</v>
@@ -1630,16 +1630,16 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1656,19 +1656,19 @@
         <v>1000</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G14" t="s">
         <v>7</v>
       </c>
       <c r="J14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1688,21 +1688,21 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B16" s="2">
         <v>700</v>
@@ -1717,16 +1717,16 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1746,21 +1746,21 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="2">
         <v>700</v>
@@ -1775,21 +1775,21 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B19" s="2">
         <v>700</v>
@@ -1804,21 +1804,21 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B20">
         <v>700</v>
@@ -1830,24 +1830,24 @@
         <v>1500</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G20" t="s">
         <v>7</v>
       </c>
       <c r="J20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B21" s="5">
         <v>800</v>
@@ -1862,21 +1862,21 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B22" s="5">
         <v>800</v>
@@ -1891,21 +1891,21 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B23" s="5">
         <v>800</v>
@@ -1920,16 +1920,16 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1946,23 +1946,23 @@
         <v>1500</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1986,15 +1986,15 @@
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>46</v>
+        <v>241</v>
       </c>
       <c r="B26" s="5">
         <v>800</v>
@@ -2013,15 +2013,15 @@
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B27" s="5">
         <v>800</v>
@@ -2033,28 +2033,28 @@
         <v>1000</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="5">
         <v>800</v>
@@ -2066,30 +2066,30 @@
         <v>1000</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B29" s="5">
         <v>800</v>
@@ -2104,21 +2104,21 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30">
         <v>800</v>
@@ -2130,21 +2130,21 @@
         <v>5000</v>
       </c>
       <c r="H30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31">
         <v>900</v>
@@ -2156,27 +2156,27 @@
         <v>2000</v>
       </c>
       <c r="E31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G31" t="s">
         <v>4</v>
       </c>
       <c r="I31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B32">
         <v>1000</v>
@@ -2188,21 +2188,21 @@
         <v>2000</v>
       </c>
       <c r="H32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B33" s="8">
         <v>900</v>
@@ -2217,14 +2217,14 @@
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I33" s="8"/>
       <c r="J33" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
         <v>10000</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
@@ -2249,18 +2249,18 @@
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B35" s="1">
         <v>1000</v>
@@ -2272,28 +2272,28 @@
         <v>10000</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="1">
         <v>1000</v>
@@ -2308,7 +2308,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>4</v>
@@ -2318,15 +2318,15 @@
         <v>1</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B37" s="1">
         <v>1000</v>
@@ -2341,16 +2341,16 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2367,10 +2367,10 @@
         <v>20000</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>4</v>
@@ -2378,15 +2378,15 @@
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B39" s="7">
         <v>1200</v>
@@ -2401,19 +2401,19 @@
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B40" s="7">
         <v>1200</v>
@@ -2431,12 +2431,12 @@
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
       <c r="K40" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B41" s="7">
         <v>1200</v>
@@ -2451,16 +2451,16 @@
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2483,10 +2483,10 @@
         <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K42" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -2512,15 +2512,15 @@
         <v>0</v>
       </c>
       <c r="J43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B44" s="4">
         <v>300</v>
@@ -2541,10 +2541,10 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -2570,10 +2570,10 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -2593,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>4</v>
@@ -2603,10 +2603,10 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -2626,7 +2626,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>4</v>
@@ -2636,10 +2636,10 @@
         <v>0</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -2659,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>4</v>
@@ -2669,10 +2669,10 @@
         <v>0</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -2698,15 +2698,15 @@
         <v>0</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B50" s="4">
         <v>300</v>
@@ -2729,15 +2729,15 @@
         <v>7</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B51" s="4">
         <v>300</v>
@@ -2758,15 +2758,15 @@
         <v>7</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B52" s="4">
         <v>300</v>
@@ -2781,7 +2781,7 @@
         <v>7</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>4</v>
@@ -2791,10 +2791,10 @@
         <v>7</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -2820,10 +2820,10 @@
         <v>0</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2849,15 +2849,15 @@
         <v>0</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B55" s="4">
         <v>300</v>
@@ -2878,10 +2878,10 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -2907,15 +2907,15 @@
         <v>0</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B57" s="4">
         <v>300</v>
@@ -2933,7 +2933,7 @@
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -2959,15 +2959,15 @@
         <v>0</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B59" s="4">
         <v>300</v>
@@ -2988,10 +2988,10 @@
         <v>0</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -3014,15 +3014,15 @@
         <v>0</v>
       </c>
       <c r="J60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K60" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B61">
         <v>300</v>
@@ -3040,10 +3040,10 @@
         <v>0</v>
       </c>
       <c r="J61" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K61" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -3069,10 +3069,10 @@
         <v>0</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -3098,10 +3098,10 @@
         <v>0</v>
       </c>
       <c r="J63" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K63" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -3127,10 +3127,10 @@
         <v>0</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -3156,10 +3156,10 @@
         <v>0</v>
       </c>
       <c r="J65" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K65" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -3176,7 +3176,7 @@
         <v>400</v>
       </c>
       <c r="E66" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F66" t="s">
         <v>0</v>
@@ -3185,18 +3185,18 @@
         <v>4</v>
       </c>
       <c r="I66" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K66" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B67" s="5">
         <v>400</v>
@@ -3211,16 +3211,16 @@
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
       <c r="H67" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K67" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -3240,16 +3240,16 @@
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
       <c r="H68" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K68" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -3269,7 +3269,7 @@
         <v>6</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>7</v>
@@ -3277,10 +3277,10 @@
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K69" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -3304,10 +3304,10 @@
       </c>
       <c r="I70" s="5"/>
       <c r="J70" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K70" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -3324,23 +3324,23 @@
         <v>800</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H71" s="5"/>
       <c r="I71" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K71" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -3364,15 +3364,15 @@
       </c>
       <c r="I72" s="5"/>
       <c r="J72" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K72" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B73">
         <v>400</v>
@@ -3384,30 +3384,30 @@
         <v>600</v>
       </c>
       <c r="E73" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F73" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G73" t="s">
         <v>4</v>
       </c>
       <c r="H73" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I73" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J73" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K73" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B74">
         <v>400</v>
@@ -3419,19 +3419,19 @@
         <v>1000</v>
       </c>
       <c r="E74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G74" t="s">
         <v>4</v>
       </c>
       <c r="I74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K74" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -3451,21 +3451,21 @@
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
       <c r="H75" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I75" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J75" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K75" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B76" s="9">
         <v>500</v>
@@ -3477,7 +3477,7 @@
         <v>1000</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F76" s="9"/>
       <c r="G76" s="9" t="s">
@@ -3485,13 +3485,13 @@
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J76" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K76" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -3508,21 +3508,21 @@
         <v>5000</v>
       </c>
       <c r="H77" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I77" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J77" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K77" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B78" s="8">
         <v>500</v>
@@ -3537,14 +3537,14 @@
       <c r="F78" s="8"/>
       <c r="G78" s="8"/>
       <c r="H78" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I78" s="8"/>
       <c r="J78" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K78" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -3561,23 +3561,23 @@
         <v>6000</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -3594,23 +3594,23 @@
         <v>6000</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -3630,7 +3630,7 @@
         <v>1</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>4</v>
@@ -3640,10 +3640,10 @@
         <v>1</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -3669,10 +3669,10 @@
         <v>1</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -3689,10 +3689,10 @@
         <v>16000</v>
       </c>
       <c r="E83" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F83" s="8" t="s">
         <v>189</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>190</v>
       </c>
       <c r="G83" s="8" t="s">
         <v>4</v>
@@ -3700,10 +3700,10 @@
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K83" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -3719,7 +3719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814E68EB-9B8B-4E2B-8BBC-E013286E9654}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -3730,21 +3730,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" t="s">
         <v>146</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>147</v>
       </c>
-      <c r="D1" t="s">
-        <v>148</v>
-      </c>
       <c r="E1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -3758,7 +3758,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3">
         <v>-50</v>
@@ -3772,7 +3772,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4">
         <v>-50</v>
@@ -3786,7 +3786,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B5">
         <v>-50</v>
@@ -3800,7 +3800,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B6">
         <v>-50</v>
@@ -3814,23 +3814,23 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B9">
         <v>30</v>
@@ -3841,7 +3841,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10">
         <v>25</v>
@@ -3855,7 +3855,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B11">
         <v>50</v>
@@ -3869,7 +3869,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B12">
         <v>50</v>
@@ -3883,7 +3883,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B13">
         <v>50</v>
@@ -3897,7 +3897,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B14">
         <v>50</v>
@@ -3935,12 +3935,12 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -3957,7 +3957,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3974,7 +3974,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3991,7 +3991,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -4008,7 +4008,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -4045,35 +4045,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" t="s">
         <v>146</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>147</v>
       </c>
-      <c r="E1" t="s">
-        <v>148</v>
-      </c>
       <c r="F1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E3">
         <v>5000</v>
@@ -4084,25 +4084,25 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E7">
         <v>5000</v>
@@ -4113,10 +4113,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
         <v>176</v>
-      </c>
-      <c r="B8" t="s">
-        <v>177</v>
       </c>
       <c r="E8">
         <v>5000</v>
@@ -4127,10 +4127,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9">
         <v>50</v>
@@ -4144,70 +4144,70 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E22">
         <v>80000</v>
@@ -4218,30 +4218,30 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C27">
         <v>50</v>
@@ -4255,10 +4255,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D28">
         <v>-4</v>
@@ -4272,50 +4272,50 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E37">
         <v>80000</v>
@@ -4326,15 +4326,15 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C39">
         <v>25</v>
@@ -4348,10 +4348,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B40" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E40">
         <v>50000</v>
@@ -4362,10 +4362,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C41">
         <v>50</v>
@@ -4379,15 +4379,15 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E43">
         <v>300</v>
@@ -4398,10 +4398,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E44">
         <v>5000</v>
@@ -4431,29 +4431,29 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" t="s">
         <v>146</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>147</v>
       </c>
-      <c r="E1" t="s">
-        <v>148</v>
-      </c>
       <c r="F1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -4461,72 +4461,72 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B14" t="s">
         <v>29</v>
@@ -4534,28 +4534,28 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18">
         <v>100</v>
@@ -4566,7 +4566,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
@@ -4580,10 +4580,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C20">
         <v>100</v>
@@ -4594,28 +4594,28 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B24" t="s">
         <v>44</v>
@@ -4623,23 +4623,23 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -4647,7 +4647,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
@@ -4655,47 +4655,47 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B29" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wolf armor has a more reasonable price
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111BB998-3095-4E9D-B8B8-AB920115D713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B059712-5FF1-42E6-8FFE-D1F6FB274FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
@@ -1234,7 +1234,7 @@
   <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2127,7 +2127,7 @@
         <v>50</v>
       </c>
       <c r="D30">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="H30" t="s">
         <v>190</v>

</xml_diff>

<commit_message>
Add Ancient Helmet of the Unfrozen
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B059712-5FF1-42E6-8FFE-D1F6FB274FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5AC855-295C-45F8-8B79-F8B5212D395A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
   <sheets>
     <sheet name="Armors" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="243">
   <si>
     <t>Leather</t>
   </si>
@@ -766,6 +766,9 @@
   </si>
   <si>
     <t>Heavy_Falmer</t>
+  </si>
+  <si>
+    <t>AncientHelmetOfTheUnfrozen</t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -4030,10 +4033,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B796E76-FF31-432C-A859-43C3EAF890A5}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4116,10 +4119,7 @@
         <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E8">
-        <v>5000</v>
+        <v>116</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -4127,141 +4127,135 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>242</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C9">
-        <v>50</v>
-      </c>
-      <c r="E9">
-        <v>80000</v>
+        <v>176</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="E10">
+        <v>80000</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" t="s">
-        <v>113</v>
-      </c>
-      <c r="E22">
-        <v>80000</v>
-      </c>
-      <c r="F22" t="b">
-        <v>1</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23">
+        <v>80000</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27" t="s">
-        <v>116</v>
-      </c>
-      <c r="C27">
-        <v>50</v>
-      </c>
-      <c r="E27">
-        <v>5000</v>
-      </c>
-      <c r="F27" t="b">
-        <v>0</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28">
-        <v>-4</v>
+        <v>116</v>
+      </c>
+      <c r="C28">
+        <v>50</v>
       </c>
       <c r="E28">
         <v>5000</v>
@@ -4272,89 +4266,92 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29">
+        <v>-4</v>
+      </c>
+      <c r="E29">
+        <v>5000</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>103</v>
-      </c>
-      <c r="B37" t="s">
-        <v>118</v>
-      </c>
-      <c r="E37">
-        <v>80000</v>
-      </c>
-      <c r="F37" t="b">
-        <v>1</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+      <c r="E38">
+        <v>80000</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>105</v>
-      </c>
-      <c r="B39" t="s">
-        <v>119</v>
-      </c>
-      <c r="C39">
-        <v>25</v>
-      </c>
-      <c r="E39">
-        <v>5000</v>
-      </c>
-      <c r="F39" t="b">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B40" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+      <c r="C40">
+        <v>25</v>
       </c>
       <c r="E40">
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
@@ -4362,51 +4359,65 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B41" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="E41">
-        <v>80000</v>
+        <v>50000</v>
       </c>
       <c r="F41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+      <c r="B42" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42">
+        <v>50</v>
+      </c>
+      <c r="E42">
+        <v>80000</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>109</v>
-      </c>
-      <c r="B43" t="s">
-        <v>122</v>
-      </c>
-      <c r="E43">
-        <v>300</v>
-      </c>
-      <c r="F43" t="b">
-        <v>0</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" t="s">
+        <v>122</v>
+      </c>
+      <c r="E44">
+        <v>300</v>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>110</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>123</v>
       </c>
-      <c r="E44">
+      <c r="E45">
         <v>5000</v>
       </c>
-      <c r="F44" t="b">
+      <c r="F45" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rework cursed dremora items
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129E3DAD-D3FC-48D9-A577-B51EA51D8D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A2DC29-D613-4008-B9D1-16C573C8307B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
   <sheets>
     <sheet name="Armors" sheetId="1" r:id="rId1"/>
@@ -1248,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="J67" sqref="J67"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2437,7 +2437,7 @@
         <v>100</v>
       </c>
       <c r="D40" s="7">
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
@@ -4047,7 +4047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B796E76-FF31-432C-A859-43C3EAF890A5}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Rework cursed dremora items (#504)
</commit_message>
<xml_diff>
--- a/tools/xEdit Scripts/patcher_data/Armor.xlsx
+++ b/tools/xEdit Scripts/patcher_data/Armor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skyrim Tools\Mod Organizer SSE\mods\requiem\tools\xEdit Scripts\patcher_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129E3DAD-D3FC-48D9-A577-B51EA51D8D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A2DC29-D613-4008-B9D1-16C573C8307B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAEF82C5-6911-4E95-BAB0-4D15EB9D7C13}"/>
   </bookViews>
   <sheets>
     <sheet name="Armors" sheetId="1" r:id="rId1"/>
@@ -1248,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34A1DA9-4FCB-4670-A236-BAEE9DAE897D}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="J67" sqref="J67"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2437,7 +2437,7 @@
         <v>100</v>
       </c>
       <c r="D40" s="7">
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
@@ -4047,7 +4047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B796E76-FF31-432C-A859-43C3EAF890A5}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>